<commit_message>
building stock collection updated
</commit_message>
<xml_diff>
--- a/projects/test_building/input/SimulatorScenarios.xlsx
+++ b/projects/test_building/input/SimulatorScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34C8F59-FDB6-644E-A764-06D1A60085B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D686194-5D8B-3043-A404-202BFA7E9E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2144,7 +2144,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
new_parallel func used and win.bat file added
</commit_message>
<xml_diff>
--- a/projects/test_building/input/SimulatorScenarios.xlsx
+++ b/projects/test_building/input/SimulatorScenarios.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yus\Documents\code\3E\RenderNew\projects\test_building\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D8CEC8-259B-2B45-9A93-A75490055078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="nuts3" sheetId="1" r:id="rId1"/>
@@ -80,8 +79,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -187,14 +186,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,69 +537,69 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:N402" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:N402" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:N402" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="A1:N402"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="start_year" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="end_year" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="id_region" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="building_num_min" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="building_num_max" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="name" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="comment" dataDxfId="0"/>
+    <tableColumn id="1" name="id" dataDxfId="29"/>
+    <tableColumn id="2" name="start_year" dataDxfId="28"/>
+    <tableColumn id="3" name="end_year" dataDxfId="27"/>
+    <tableColumn id="4" name="id_region" dataDxfId="26"/>
+    <tableColumn id="5" name="building_num_min" dataDxfId="25"/>
+    <tableColumn id="6" name="building_num_max" dataDxfId="24"/>
+    <tableColumn id="7" name="optimal_heating_behavior_prob" dataDxfId="23"/>
+    <tableColumn id="8" name="id_scenario_energy_price_wholesale" dataDxfId="22"/>
+    <tableColumn id="9" name="id_scenario_energy_price_tax_rate" dataDxfId="21"/>
+    <tableColumn id="10" name="id_scenario_energy_price_mark_up" dataDxfId="20"/>
+    <tableColumn id="11" name="id_scenario_energy_price_co2_emission" dataDxfId="19"/>
+    <tableColumn id="12" name="id_scenario_energy_emission_factor" dataDxfId="18"/>
+    <tableColumn id="13" name="name" dataDxfId="17"/>
+    <tableColumn id="14" name="comment" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:N2" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A1:N2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:N2" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:N2"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="start_year" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="end_year" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_region" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="building_num_min" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="building_num_max" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="name" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="comment" dataDxfId="16"/>
+    <tableColumn id="1" name="id" dataDxfId="13"/>
+    <tableColumn id="2" name="start_year" dataDxfId="12"/>
+    <tableColumn id="3" name="end_year" dataDxfId="11"/>
+    <tableColumn id="4" name="id_region" dataDxfId="10"/>
+    <tableColumn id="5" name="building_num_min" dataDxfId="9"/>
+    <tableColumn id="6" name="building_num_max" dataDxfId="8"/>
+    <tableColumn id="7" name="optimal_heating_behavior_prob" dataDxfId="7"/>
+    <tableColumn id="8" name="id_scenario_energy_price_wholesale" dataDxfId="6"/>
+    <tableColumn id="9" name="id_scenario_energy_price_tax_rate" dataDxfId="5"/>
+    <tableColumn id="10" name="id_scenario_energy_price_mark_up" dataDxfId="4"/>
+    <tableColumn id="11" name="id_scenario_energy_price_co2_emission" dataDxfId="3"/>
+    <tableColumn id="12" name="id_scenario_energy_emission_factor" dataDxfId="2"/>
+    <tableColumn id="13" name="name" dataDxfId="1"/>
+    <tableColumn id="14" name="comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="A1:N27" totalsRowShown="0">
-  <autoFilter ref="A1:N27" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:N27" totalsRowShown="0">
+  <autoFilter ref="A1:N27"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="start_year"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="end_year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="id_region"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="building_num_min"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="building_num_max"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="optimal_heating_behavior_prob"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="id_scenario_energy_price_wholesale"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="id_scenario_energy_price_tax_rate"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="id_scenario_energy_price_mark_up"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="id_scenario_energy_price_co2_emission"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="id_scenario_energy_emission_factor"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="name"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="comment"/>
+    <tableColumn id="1" name="id"/>
+    <tableColumn id="2" name="start_year"/>
+    <tableColumn id="3" name="end_year"/>
+    <tableColumn id="4" name="id_region"/>
+    <tableColumn id="5" name="building_num_min"/>
+    <tableColumn id="6" name="building_num_max"/>
+    <tableColumn id="7" name="optimal_heating_behavior_prob"/>
+    <tableColumn id="8" name="id_scenario_energy_price_wholesale"/>
+    <tableColumn id="9" name="id_scenario_energy_price_tax_rate"/>
+    <tableColumn id="10" name="id_scenario_energy_price_mark_up"/>
+    <tableColumn id="11" name="id_scenario_energy_price_co2_emission"/>
+    <tableColumn id="12" name="id_scenario_energy_emission_factor"/>
+    <tableColumn id="13" name="name"/>
+    <tableColumn id="14" name="comment"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -868,26 +867,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N402"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" customWidth="1"/>
-    <col min="7" max="7" width="32.5" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" customWidth="1"/>
     <col min="8" max="12" width="32" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -931,7 +930,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -975,7 +974,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -1019,7 +1018,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -1063,7 +1062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="11">
         <v>1</v>
       </c>
@@ -1107,7 +1106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="11">
         <v>1</v>
       </c>
@@ -1151,7 +1150,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="11">
         <v>1</v>
       </c>
@@ -1195,7 +1194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="11">
         <v>1</v>
       </c>
@@ -1239,7 +1238,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="11">
         <v>1</v>
       </c>
@@ -1283,7 +1282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" s="11">
         <v>1</v>
       </c>
@@ -1327,7 +1326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" s="11">
         <v>1</v>
       </c>
@@ -1371,7 +1370,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" s="11">
         <v>1</v>
       </c>
@@ -1415,7 +1414,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" s="11">
         <v>1</v>
       </c>
@@ -1459,7 +1458,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" s="11">
         <v>1</v>
       </c>
@@ -1503,7 +1502,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="A15" s="11">
         <v>1</v>
       </c>
@@ -1547,7 +1546,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" s="11">
         <v>1</v>
       </c>
@@ -1591,7 +1590,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14">
       <c r="A17" s="11">
         <v>1</v>
       </c>
@@ -1635,7 +1634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14">
       <c r="A18" s="11">
         <v>1</v>
       </c>
@@ -1679,7 +1678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14">
       <c r="A19" s="11">
         <v>1</v>
       </c>
@@ -1723,7 +1722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14">
       <c r="A20" s="11">
         <v>1</v>
       </c>
@@ -1767,7 +1766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14">
       <c r="A21" s="11">
         <v>1</v>
       </c>
@@ -1811,7 +1810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14">
       <c r="A22" s="11">
         <v>1</v>
       </c>
@@ -1855,7 +1854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14">
       <c r="A23" s="11">
         <v>1</v>
       </c>
@@ -1899,7 +1898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14">
       <c r="A24" s="11">
         <v>1</v>
       </c>
@@ -1943,7 +1942,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14">
       <c r="A25" s="11">
         <v>1</v>
       </c>
@@ -1987,7 +1986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14">
       <c r="A26" s="11">
         <v>1</v>
       </c>
@@ -2031,7 +2030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14">
       <c r="A27" s="11">
         <v>1</v>
       </c>
@@ -2075,7 +2074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14">
       <c r="A28" s="11">
         <v>1</v>
       </c>
@@ -2119,7 +2118,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14">
       <c r="A29" s="11">
         <v>1</v>
       </c>
@@ -2163,7 +2162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14">
       <c r="A30" s="11">
         <v>1</v>
       </c>
@@ -2207,7 +2206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14">
       <c r="A31" s="11">
         <v>1</v>
       </c>
@@ -2251,7 +2250,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14">
       <c r="A32" s="11">
         <v>1</v>
       </c>
@@ -2295,7 +2294,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14">
       <c r="A33" s="11">
         <v>1</v>
       </c>
@@ -2339,7 +2338,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14">
       <c r="A34" s="11">
         <v>1</v>
       </c>
@@ -2383,7 +2382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14">
       <c r="A35" s="11">
         <v>1</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14">
       <c r="A36" s="11">
         <v>1</v>
       </c>
@@ -2471,7 +2470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14">
       <c r="A37" s="11">
         <v>1</v>
       </c>
@@ -2515,7 +2514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14">
       <c r="A38" s="11">
         <v>1</v>
       </c>
@@ -2559,7 +2558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14">
       <c r="A39" s="11">
         <v>1</v>
       </c>
@@ -2603,7 +2602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14">
       <c r="A40" s="11">
         <v>1</v>
       </c>
@@ -2647,7 +2646,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14">
       <c r="A41" s="11">
         <v>1</v>
       </c>
@@ -2691,7 +2690,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14">
       <c r="A42" s="11">
         <v>1</v>
       </c>
@@ -2735,7 +2734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14">
       <c r="A43" s="11">
         <v>1</v>
       </c>
@@ -2779,7 +2778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14">
       <c r="A44" s="11">
         <v>1</v>
       </c>
@@ -2823,7 +2822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14">
       <c r="A45" s="11">
         <v>1</v>
       </c>
@@ -2867,7 +2866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14">
       <c r="A46" s="11">
         <v>1</v>
       </c>
@@ -2911,7 +2910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14">
       <c r="A47" s="11">
         <v>1</v>
       </c>
@@ -2955,7 +2954,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14">
       <c r="A48" s="11">
         <v>1</v>
       </c>
@@ -2999,7 +2998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14">
       <c r="A49" s="11">
         <v>1</v>
       </c>
@@ -3043,7 +3042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14">
       <c r="A50" s="11">
         <v>1</v>
       </c>
@@ -3087,7 +3086,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14">
       <c r="A51" s="11">
         <v>1</v>
       </c>
@@ -3131,7 +3130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14">
       <c r="A52" s="11">
         <v>1</v>
       </c>
@@ -3175,7 +3174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14">
       <c r="A53" s="11">
         <v>1</v>
       </c>
@@ -3219,7 +3218,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14">
       <c r="A54" s="11">
         <v>1</v>
       </c>
@@ -3263,7 +3262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14">
       <c r="A55" s="11">
         <v>1</v>
       </c>
@@ -3307,7 +3306,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14">
       <c r="A56" s="11">
         <v>1</v>
       </c>
@@ -3351,7 +3350,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14">
       <c r="A57" s="11">
         <v>1</v>
       </c>
@@ -3395,7 +3394,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14">
       <c r="A58" s="11">
         <v>1</v>
       </c>
@@ -3439,7 +3438,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14">
       <c r="A59" s="11">
         <v>1</v>
       </c>
@@ -3483,7 +3482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14">
       <c r="A60" s="11">
         <v>1</v>
       </c>
@@ -3527,7 +3526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14">
       <c r="A61" s="11">
         <v>1</v>
       </c>
@@ -3571,7 +3570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14">
       <c r="A62" s="11">
         <v>1</v>
       </c>
@@ -3615,7 +3614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14">
       <c r="A63" s="11">
         <v>1</v>
       </c>
@@ -3659,7 +3658,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14">
       <c r="A64" s="11">
         <v>1</v>
       </c>
@@ -3703,7 +3702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14">
       <c r="A65" s="11">
         <v>1</v>
       </c>
@@ -3747,7 +3746,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14">
       <c r="A66" s="11">
         <v>1</v>
       </c>
@@ -3791,7 +3790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14">
       <c r="A67" s="11">
         <v>1</v>
       </c>
@@ -3835,7 +3834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14">
       <c r="A68" s="11">
         <v>1</v>
       </c>
@@ -3879,7 +3878,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14">
       <c r="A69" s="11">
         <v>1</v>
       </c>
@@ -3923,7 +3922,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14">
       <c r="A70" s="11">
         <v>1</v>
       </c>
@@ -3967,7 +3966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14">
       <c r="A71" s="11">
         <v>1</v>
       </c>
@@ -4011,7 +4010,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14">
       <c r="A72" s="11">
         <v>1</v>
       </c>
@@ -4055,7 +4054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14">
       <c r="A73" s="11">
         <v>1</v>
       </c>
@@ -4099,7 +4098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14">
       <c r="A74" s="11">
         <v>1</v>
       </c>
@@ -4143,7 +4142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14">
       <c r="A75" s="11">
         <v>1</v>
       </c>
@@ -4187,7 +4186,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14">
       <c r="A76" s="11">
         <v>1</v>
       </c>
@@ -4231,7 +4230,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14">
       <c r="A77" s="11">
         <v>1</v>
       </c>
@@ -4275,7 +4274,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14">
       <c r="A78" s="11">
         <v>1</v>
       </c>
@@ -4319,7 +4318,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14">
       <c r="A79" s="11">
         <v>1</v>
       </c>
@@ -4363,7 +4362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14">
       <c r="A80" s="11">
         <v>1</v>
       </c>
@@ -4407,7 +4406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14">
       <c r="A81" s="11">
         <v>1</v>
       </c>
@@ -4451,7 +4450,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14">
       <c r="A82" s="11">
         <v>1</v>
       </c>
@@ -4495,7 +4494,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14">
       <c r="A83" s="11">
         <v>1</v>
       </c>
@@ -4539,7 +4538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14">
       <c r="A84" s="11">
         <v>1</v>
       </c>
@@ -4583,7 +4582,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14">
       <c r="A85" s="11">
         <v>1</v>
       </c>
@@ -4627,7 +4626,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14">
       <c r="A86" s="11">
         <v>1</v>
       </c>
@@ -4671,7 +4670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14">
       <c r="A87" s="11">
         <v>1</v>
       </c>
@@ -4715,7 +4714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14">
       <c r="A88" s="11">
         <v>1</v>
       </c>
@@ -4759,7 +4758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14">
       <c r="A89" s="11">
         <v>1</v>
       </c>
@@ -4803,7 +4802,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14">
       <c r="A90" s="11">
         <v>1</v>
       </c>
@@ -4847,7 +4846,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14">
       <c r="A91" s="11">
         <v>1</v>
       </c>
@@ -4891,7 +4890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14">
       <c r="A92" s="11">
         <v>1</v>
       </c>
@@ -4935,7 +4934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14">
       <c r="A93" s="11">
         <v>1</v>
       </c>
@@ -4979,7 +4978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14">
       <c r="A94" s="11">
         <v>1</v>
       </c>
@@ -5023,7 +5022,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14">
       <c r="A95" s="11">
         <v>1</v>
       </c>
@@ -5067,7 +5066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14">
       <c r="A96" s="11">
         <v>1</v>
       </c>
@@ -5111,7 +5110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14">
       <c r="A97" s="11">
         <v>1</v>
       </c>
@@ -5155,7 +5154,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14">
       <c r="A98" s="11">
         <v>1</v>
       </c>
@@ -5199,7 +5198,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14">
       <c r="A99" s="11">
         <v>1</v>
       </c>
@@ -5243,7 +5242,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14">
       <c r="A100" s="11">
         <v>1</v>
       </c>
@@ -5287,7 +5286,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14">
       <c r="A101" s="11">
         <v>1</v>
       </c>
@@ -5331,7 +5330,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14">
       <c r="A102" s="11">
         <v>1</v>
       </c>
@@ -5375,7 +5374,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14">
       <c r="A103" s="11">
         <v>1</v>
       </c>
@@ -5419,7 +5418,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14">
       <c r="A104" s="11">
         <v>1</v>
       </c>
@@ -5463,7 +5462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14">
       <c r="A105" s="11">
         <v>1</v>
       </c>
@@ -5507,7 +5506,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14">
       <c r="A106" s="11">
         <v>1</v>
       </c>
@@ -5551,7 +5550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14">
       <c r="A107" s="11">
         <v>1</v>
       </c>
@@ -5595,7 +5594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14">
       <c r="A108" s="11">
         <v>1</v>
       </c>
@@ -5639,7 +5638,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14">
       <c r="A109" s="11">
         <v>1</v>
       </c>
@@ -5683,7 +5682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14">
       <c r="A110" s="11">
         <v>1</v>
       </c>
@@ -5727,7 +5726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14">
       <c r="A111" s="11">
         <v>1</v>
       </c>
@@ -5771,7 +5770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14">
       <c r="A112" s="11">
         <v>1</v>
       </c>
@@ -5815,7 +5814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14">
       <c r="A113" s="11">
         <v>1</v>
       </c>
@@ -5859,7 +5858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14">
       <c r="A114" s="11">
         <v>1</v>
       </c>
@@ -5903,7 +5902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14">
       <c r="A115" s="11">
         <v>1</v>
       </c>
@@ -5947,7 +5946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14">
       <c r="A116" s="11">
         <v>1</v>
       </c>
@@ -5991,7 +5990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14">
       <c r="A117" s="11">
         <v>1</v>
       </c>
@@ -6035,7 +6034,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14">
       <c r="A118" s="11">
         <v>1</v>
       </c>
@@ -6079,7 +6078,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14">
       <c r="A119" s="11">
         <v>1</v>
       </c>
@@ -6123,7 +6122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14">
       <c r="A120" s="11">
         <v>1</v>
       </c>
@@ -6167,7 +6166,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14">
       <c r="A121" s="11">
         <v>1</v>
       </c>
@@ -6211,7 +6210,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14">
       <c r="A122" s="11">
         <v>1</v>
       </c>
@@ -6255,7 +6254,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14">
       <c r="A123" s="11">
         <v>1</v>
       </c>
@@ -6299,7 +6298,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14">
       <c r="A124" s="11">
         <v>1</v>
       </c>
@@ -6343,7 +6342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14">
       <c r="A125" s="11">
         <v>1</v>
       </c>
@@ -6387,7 +6386,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14">
       <c r="A126" s="11">
         <v>1</v>
       </c>
@@ -6431,7 +6430,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14">
       <c r="A127" s="11">
         <v>1</v>
       </c>
@@ -6475,7 +6474,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14">
       <c r="A128" s="11">
         <v>1</v>
       </c>
@@ -6519,7 +6518,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14">
       <c r="A129" s="11">
         <v>1</v>
       </c>
@@ -6563,7 +6562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:14">
       <c r="A130" s="11">
         <v>1</v>
       </c>
@@ -6607,7 +6606,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:14">
       <c r="A131" s="11">
         <v>1</v>
       </c>
@@ -6651,7 +6650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:14">
       <c r="A132" s="11">
         <v>1</v>
       </c>
@@ -6695,7 +6694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:14">
       <c r="A133" s="11">
         <v>1</v>
       </c>
@@ -6739,7 +6738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:14">
       <c r="A134" s="11">
         <v>1</v>
       </c>
@@ -6783,7 +6782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:14">
       <c r="A135" s="11">
         <v>1</v>
       </c>
@@ -6827,7 +6826,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:14">
       <c r="A136" s="11">
         <v>1</v>
       </c>
@@ -6871,7 +6870,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:14">
       <c r="A137" s="11">
         <v>1</v>
       </c>
@@ -6915,7 +6914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:14">
       <c r="A138" s="11">
         <v>1</v>
       </c>
@@ -6959,7 +6958,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:14">
       <c r="A139" s="11">
         <v>1</v>
       </c>
@@ -7003,7 +7002,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:14">
       <c r="A140" s="11">
         <v>1</v>
       </c>
@@ -7047,7 +7046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:14">
       <c r="A141" s="11">
         <v>1</v>
       </c>
@@ -7091,7 +7090,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:14">
       <c r="A142" s="11">
         <v>1</v>
       </c>
@@ -7135,7 +7134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:14">
       <c r="A143" s="11">
         <v>1</v>
       </c>
@@ -7179,7 +7178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:14">
       <c r="A144" s="11">
         <v>1</v>
       </c>
@@ -7223,7 +7222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:14">
       <c r="A145" s="11">
         <v>1</v>
       </c>
@@ -7267,7 +7266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:14">
       <c r="A146" s="11">
         <v>1</v>
       </c>
@@ -7311,7 +7310,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:14">
       <c r="A147" s="11">
         <v>1</v>
       </c>
@@ -7355,7 +7354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:14">
       <c r="A148" s="11">
         <v>1</v>
       </c>
@@ -7399,7 +7398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:14">
       <c r="A149" s="11">
         <v>1</v>
       </c>
@@ -7443,7 +7442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:14">
       <c r="A150" s="11">
         <v>1</v>
       </c>
@@ -7487,7 +7486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:14">
       <c r="A151" s="11">
         <v>1</v>
       </c>
@@ -7531,7 +7530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:14">
       <c r="A152" s="11">
         <v>1</v>
       </c>
@@ -7575,7 +7574,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:14">
       <c r="A153" s="11">
         <v>1</v>
       </c>
@@ -7619,7 +7618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:14">
       <c r="A154" s="11">
         <v>1</v>
       </c>
@@ -7663,7 +7662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:14">
       <c r="A155" s="11">
         <v>1</v>
       </c>
@@ -7707,7 +7706,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:14">
       <c r="A156" s="11">
         <v>1</v>
       </c>
@@ -7751,7 +7750,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:14">
       <c r="A157" s="11">
         <v>1</v>
       </c>
@@ -7795,7 +7794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:14">
       <c r="A158" s="11">
         <v>1</v>
       </c>
@@ -7839,7 +7838,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:14">
       <c r="A159" s="11">
         <v>1</v>
       </c>
@@ -7883,7 +7882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:14">
       <c r="A160" s="11">
         <v>1</v>
       </c>
@@ -7927,7 +7926,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:14">
       <c r="A161" s="11">
         <v>1</v>
       </c>
@@ -7971,7 +7970,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:14">
       <c r="A162" s="11">
         <v>1</v>
       </c>
@@ -8015,7 +8014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:14">
       <c r="A163" s="11">
         <v>1</v>
       </c>
@@ -8059,7 +8058,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:14">
       <c r="A164" s="11">
         <v>1</v>
       </c>
@@ -8103,7 +8102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:14">
       <c r="A165" s="11">
         <v>1</v>
       </c>
@@ -8147,7 +8146,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:14">
       <c r="A166" s="11">
         <v>1</v>
       </c>
@@ -8191,7 +8190,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:14">
       <c r="A167" s="11">
         <v>1</v>
       </c>
@@ -8235,7 +8234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:14">
       <c r="A168" s="11">
         <v>1</v>
       </c>
@@ -8279,7 +8278,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:14">
       <c r="A169" s="11">
         <v>1</v>
       </c>
@@ -8323,7 +8322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:14">
       <c r="A170" s="11">
         <v>1</v>
       </c>
@@ -8367,7 +8366,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:14">
       <c r="A171" s="11">
         <v>1</v>
       </c>
@@ -8411,7 +8410,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:14">
       <c r="A172" s="11">
         <v>1</v>
       </c>
@@ -8455,7 +8454,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:14">
       <c r="A173" s="11">
         <v>1</v>
       </c>
@@ -8499,7 +8498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:14">
       <c r="A174" s="11">
         <v>1</v>
       </c>
@@ -8543,7 +8542,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:14">
       <c r="A175" s="11">
         <v>1</v>
       </c>
@@ -8587,7 +8586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:14">
       <c r="A176" s="11">
         <v>1</v>
       </c>
@@ -8631,7 +8630,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:14">
       <c r="A177" s="11">
         <v>1</v>
       </c>
@@ -8675,7 +8674,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:14">
       <c r="A178" s="11">
         <v>1</v>
       </c>
@@ -8719,7 +8718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:14">
       <c r="A179" s="11">
         <v>1</v>
       </c>
@@ -8763,7 +8762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:14">
       <c r="A180" s="11">
         <v>1</v>
       </c>
@@ -8807,7 +8806,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:14">
       <c r="A181" s="11">
         <v>1</v>
       </c>
@@ -8851,7 +8850,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:14">
       <c r="A182" s="11">
         <v>1</v>
       </c>
@@ -8895,7 +8894,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:14">
       <c r="A183" s="11">
         <v>1</v>
       </c>
@@ -8939,7 +8938,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:14">
       <c r="A184" s="11">
         <v>1</v>
       </c>
@@ -8983,7 +8982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:14">
       <c r="A185" s="11">
         <v>1</v>
       </c>
@@ -9027,7 +9026,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:14">
       <c r="A186" s="11">
         <v>1</v>
       </c>
@@ -9071,7 +9070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:14">
       <c r="A187" s="11">
         <v>1</v>
       </c>
@@ -9115,7 +9114,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:14">
       <c r="A188" s="11">
         <v>1</v>
       </c>
@@ -9159,7 +9158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:14">
       <c r="A189" s="11">
         <v>1</v>
       </c>
@@ -9203,7 +9202,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:14">
       <c r="A190" s="11">
         <v>1</v>
       </c>
@@ -9247,7 +9246,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:14">
       <c r="A191" s="11">
         <v>1</v>
       </c>
@@ -9291,7 +9290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:14">
       <c r="A192" s="11">
         <v>1</v>
       </c>
@@ -9335,7 +9334,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:14">
       <c r="A193" s="11">
         <v>1</v>
       </c>
@@ -9379,7 +9378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:14">
       <c r="A194" s="11">
         <v>1</v>
       </c>
@@ -9423,7 +9422,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:14">
       <c r="A195" s="11">
         <v>1</v>
       </c>
@@ -9467,7 +9466,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:14">
       <c r="A196" s="11">
         <v>1</v>
       </c>
@@ -9511,7 +9510,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:14">
       <c r="A197" s="11">
         <v>1</v>
       </c>
@@ -9555,7 +9554,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:14">
       <c r="A198" s="11">
         <v>1</v>
       </c>
@@ -9599,7 +9598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:14">
       <c r="A199" s="11">
         <v>1</v>
       </c>
@@ -9643,7 +9642,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:14">
       <c r="A200" s="11">
         <v>1</v>
       </c>
@@ -9687,7 +9686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:14">
       <c r="A201" s="11">
         <v>1</v>
       </c>
@@ -9731,7 +9730,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:14">
       <c r="A202" s="11">
         <v>1</v>
       </c>
@@ -9775,7 +9774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:14">
       <c r="A203" s="11">
         <v>1</v>
       </c>
@@ -9819,7 +9818,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:14">
       <c r="A204" s="11">
         <v>1</v>
       </c>
@@ -9863,7 +9862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:14">
       <c r="A205" s="11">
         <v>1</v>
       </c>
@@ -9907,7 +9906,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:14">
       <c r="A206" s="11">
         <v>1</v>
       </c>
@@ -9951,7 +9950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:14">
       <c r="A207" s="11">
         <v>1</v>
       </c>
@@ -9995,7 +9994,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:14">
       <c r="A208" s="11">
         <v>1</v>
       </c>
@@ -10039,7 +10038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:14">
       <c r="A209" s="11">
         <v>1</v>
       </c>
@@ -10083,7 +10082,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:14">
       <c r="A210" s="11">
         <v>1</v>
       </c>
@@ -10127,7 +10126,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:14">
       <c r="A211" s="11">
         <v>1</v>
       </c>
@@ -10171,7 +10170,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:14">
       <c r="A212" s="11">
         <v>1</v>
       </c>
@@ -10215,7 +10214,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:14">
       <c r="A213" s="11">
         <v>1</v>
       </c>
@@ -10259,7 +10258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:14">
       <c r="A214" s="11">
         <v>1</v>
       </c>
@@ -10303,7 +10302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:14">
       <c r="A215" s="11">
         <v>1</v>
       </c>
@@ -10347,7 +10346,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:14">
       <c r="A216" s="11">
         <v>1</v>
       </c>
@@ -10391,7 +10390,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:14">
       <c r="A217" s="11">
         <v>1</v>
       </c>
@@ -10435,7 +10434,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:14">
       <c r="A218" s="11">
         <v>1</v>
       </c>
@@ -10479,7 +10478,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:14">
       <c r="A219" s="11">
         <v>1</v>
       </c>
@@ -10523,7 +10522,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:14">
       <c r="A220" s="11">
         <v>1</v>
       </c>
@@ -10567,7 +10566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:14">
       <c r="A221" s="11">
         <v>1</v>
       </c>
@@ -10611,7 +10610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:14">
       <c r="A222" s="11">
         <v>1</v>
       </c>
@@ -10655,7 +10654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:14">
       <c r="A223" s="11">
         <v>1</v>
       </c>
@@ -10699,7 +10698,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:14">
       <c r="A224" s="11">
         <v>1</v>
       </c>
@@ -10743,7 +10742,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:14">
       <c r="A225" s="11">
         <v>1</v>
       </c>
@@ -10787,7 +10786,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:14">
       <c r="A226" s="11">
         <v>1</v>
       </c>
@@ -10831,7 +10830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:14">
       <c r="A227" s="11">
         <v>1</v>
       </c>
@@ -10875,7 +10874,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:14">
       <c r="A228" s="11">
         <v>1</v>
       </c>
@@ -10919,7 +10918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:14">
       <c r="A229" s="11">
         <v>1</v>
       </c>
@@ -10963,7 +10962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:14">
       <c r="A230" s="11">
         <v>1</v>
       </c>
@@ -11007,7 +11006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:14">
       <c r="A231" s="11">
         <v>1</v>
       </c>
@@ -11051,7 +11050,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:14">
       <c r="A232" s="11">
         <v>1</v>
       </c>
@@ -11095,7 +11094,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:14">
       <c r="A233" s="11">
         <v>1</v>
       </c>
@@ -11139,7 +11138,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:14">
       <c r="A234" s="11">
         <v>1</v>
       </c>
@@ -11183,7 +11182,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:14">
       <c r="A235" s="11">
         <v>1</v>
       </c>
@@ -11227,7 +11226,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:14">
       <c r="A236" s="11">
         <v>1</v>
       </c>
@@ -11271,7 +11270,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:14">
       <c r="A237" s="11">
         <v>1</v>
       </c>
@@ -11315,7 +11314,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:14">
       <c r="A238" s="11">
         <v>1</v>
       </c>
@@ -11359,7 +11358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:14">
       <c r="A239" s="11">
         <v>1</v>
       </c>
@@ -11403,7 +11402,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:14">
       <c r="A240" s="11">
         <v>1</v>
       </c>
@@ -11447,7 +11446,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="241" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:14">
       <c r="A241" s="11">
         <v>1</v>
       </c>
@@ -11491,7 +11490,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="242" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:14">
       <c r="A242" s="11">
         <v>1</v>
       </c>
@@ -11535,7 +11534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="243" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:14">
       <c r="A243" s="11">
         <v>1</v>
       </c>
@@ -11579,7 +11578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:14">
       <c r="A244" s="11">
         <v>1</v>
       </c>
@@ -11623,7 +11622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="245" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:14">
       <c r="A245" s="11">
         <v>1</v>
       </c>
@@ -11667,7 +11666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:14">
       <c r="A246" s="11">
         <v>1</v>
       </c>
@@ -11711,7 +11710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="247" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:14">
       <c r="A247" s="11">
         <v>1</v>
       </c>
@@ -11755,7 +11754,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:14">
       <c r="A248" s="11">
         <v>1</v>
       </c>
@@ -11799,7 +11798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:14">
       <c r="A249" s="11">
         <v>1</v>
       </c>
@@ -11843,7 +11842,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:14">
       <c r="A250" s="11">
         <v>1</v>
       </c>
@@ -11887,7 +11886,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="251" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:14">
       <c r="A251" s="11">
         <v>1</v>
       </c>
@@ -11931,7 +11930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="252" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:14">
       <c r="A252" s="11">
         <v>1</v>
       </c>
@@ -11975,7 +11974,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="253" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:14">
       <c r="A253" s="11">
         <v>1</v>
       </c>
@@ -12019,7 +12018,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:14">
       <c r="A254" s="11">
         <v>1</v>
       </c>
@@ -12063,7 +12062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:14">
       <c r="A255" s="11">
         <v>1</v>
       </c>
@@ -12107,7 +12106,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="256" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:14">
       <c r="A256" s="11">
         <v>1</v>
       </c>
@@ -12151,7 +12150,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:14">
       <c r="A257" s="11">
         <v>1</v>
       </c>
@@ -12195,7 +12194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:14">
       <c r="A258" s="11">
         <v>1</v>
       </c>
@@ -12239,7 +12238,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="259" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:14">
       <c r="A259" s="11">
         <v>1</v>
       </c>
@@ -12283,7 +12282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="260" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:14">
       <c r="A260" s="11">
         <v>1</v>
       </c>
@@ -12327,7 +12326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="261" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:14">
       <c r="A261" s="11">
         <v>1</v>
       </c>
@@ -12371,7 +12370,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:14">
       <c r="A262" s="11">
         <v>1</v>
       </c>
@@ -12415,7 +12414,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="263" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:14">
       <c r="A263" s="11">
         <v>1</v>
       </c>
@@ -12459,7 +12458,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:14">
       <c r="A264" s="11">
         <v>1</v>
       </c>
@@ -12503,7 +12502,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="265" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:14">
       <c r="A265" s="11">
         <v>1</v>
       </c>
@@ -12547,7 +12546,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="266" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:14">
       <c r="A266" s="11">
         <v>1</v>
       </c>
@@ -12591,7 +12590,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="267" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:14">
       <c r="A267" s="11">
         <v>1</v>
       </c>
@@ -12635,7 +12634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="268" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:14">
       <c r="A268" s="11">
         <v>1</v>
       </c>
@@ -12679,7 +12678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="269" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:14">
       <c r="A269" s="11">
         <v>1</v>
       </c>
@@ -12723,7 +12722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="270" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:14">
       <c r="A270" s="11">
         <v>1</v>
       </c>
@@ -12767,7 +12766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="271" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:14">
       <c r="A271" s="11">
         <v>1</v>
       </c>
@@ -12811,7 +12810,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="272" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:14">
       <c r="A272" s="11">
         <v>1</v>
       </c>
@@ -12855,7 +12854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="273" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:14">
       <c r="A273" s="11">
         <v>1</v>
       </c>
@@ -12899,7 +12898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="274" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:14">
       <c r="A274" s="11">
         <v>1</v>
       </c>
@@ -12943,7 +12942,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="275" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:14">
       <c r="A275" s="11">
         <v>1</v>
       </c>
@@ -12987,7 +12986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="276" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:14">
       <c r="A276" s="11">
         <v>1</v>
       </c>
@@ -13031,7 +13030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="277" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:14">
       <c r="A277" s="11">
         <v>1</v>
       </c>
@@ -13075,7 +13074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="278" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:14">
       <c r="A278" s="11">
         <v>1</v>
       </c>
@@ -13119,7 +13118,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="279" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:14">
       <c r="A279" s="11">
         <v>1</v>
       </c>
@@ -13163,7 +13162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="280" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:14">
       <c r="A280" s="11">
         <v>1</v>
       </c>
@@ -13207,7 +13206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="281" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:14">
       <c r="A281" s="11">
         <v>1</v>
       </c>
@@ -13251,7 +13250,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="282" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:14">
       <c r="A282" s="11">
         <v>1</v>
       </c>
@@ -13295,7 +13294,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="283" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:14">
       <c r="A283" s="11">
         <v>1</v>
       </c>
@@ -13339,7 +13338,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="284" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:14">
       <c r="A284" s="11">
         <v>1</v>
       </c>
@@ -13383,7 +13382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="285" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:14">
       <c r="A285" s="11">
         <v>1</v>
       </c>
@@ -13427,7 +13426,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="286" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:14">
       <c r="A286" s="11">
         <v>1</v>
       </c>
@@ -13471,7 +13470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="287" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:14">
       <c r="A287" s="11">
         <v>1</v>
       </c>
@@ -13515,7 +13514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="288" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:14">
       <c r="A288" s="11">
         <v>1</v>
       </c>
@@ -13559,7 +13558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:14">
       <c r="A289" s="11">
         <v>1</v>
       </c>
@@ -13603,7 +13602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:14">
       <c r="A290" s="11">
         <v>1</v>
       </c>
@@ -13647,7 +13646,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="291" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:14">
       <c r="A291" s="11">
         <v>1</v>
       </c>
@@ -13691,7 +13690,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="292" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:14">
       <c r="A292" s="11">
         <v>1</v>
       </c>
@@ -13735,7 +13734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="293" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:14">
       <c r="A293" s="11">
         <v>1</v>
       </c>
@@ -13779,7 +13778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="294" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:14">
       <c r="A294" s="11">
         <v>1</v>
       </c>
@@ -13823,7 +13822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="295" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:14">
       <c r="A295" s="11">
         <v>1</v>
       </c>
@@ -13867,7 +13866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="296" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:14">
       <c r="A296" s="11">
         <v>1</v>
       </c>
@@ -13911,7 +13910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="297" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:14">
       <c r="A297" s="11">
         <v>1</v>
       </c>
@@ -13955,7 +13954,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="298" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:14">
       <c r="A298" s="11">
         <v>1</v>
       </c>
@@ -13999,7 +13998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="299" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:14">
       <c r="A299" s="11">
         <v>1</v>
       </c>
@@ -14043,7 +14042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:14">
       <c r="A300" s="11">
         <v>1</v>
       </c>
@@ -14087,7 +14086,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="301" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:14">
       <c r="A301" s="11">
         <v>1</v>
       </c>
@@ -14131,7 +14130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="302" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:14">
       <c r="A302" s="11">
         <v>1</v>
       </c>
@@ -14175,7 +14174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="303" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:14">
       <c r="A303" s="11">
         <v>1</v>
       </c>
@@ -14219,7 +14218,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="304" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:14">
       <c r="A304" s="11">
         <v>1</v>
       </c>
@@ -14263,7 +14262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="305" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:14">
       <c r="A305" s="11">
         <v>1</v>
       </c>
@@ -14307,7 +14306,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="306" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:14">
       <c r="A306" s="11">
         <v>1</v>
       </c>
@@ -14351,7 +14350,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="307" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:14">
       <c r="A307" s="11">
         <v>1</v>
       </c>
@@ -14395,7 +14394,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="308" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:14">
       <c r="A308" s="11">
         <v>1</v>
       </c>
@@ -14439,7 +14438,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:14">
       <c r="A309" s="11">
         <v>1</v>
       </c>
@@ -14483,7 +14482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="310" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:14">
       <c r="A310" s="11">
         <v>1</v>
       </c>
@@ -14527,7 +14526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="311" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:14">
       <c r="A311" s="11">
         <v>1</v>
       </c>
@@ -14571,7 +14570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="312" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:14">
       <c r="A312" s="11">
         <v>1</v>
       </c>
@@ -14615,7 +14614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="313" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:14">
       <c r="A313" s="11">
         <v>1</v>
       </c>
@@ -14659,7 +14658,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="314" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:14">
       <c r="A314" s="11">
         <v>1</v>
       </c>
@@ -14703,7 +14702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="315" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:14">
       <c r="A315" s="11">
         <v>1</v>
       </c>
@@ -14747,7 +14746,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="316" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:14">
       <c r="A316" s="11">
         <v>1</v>
       </c>
@@ -14791,7 +14790,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="317" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:14">
       <c r="A317" s="11">
         <v>1</v>
       </c>
@@ -14835,7 +14834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="318" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:14">
       <c r="A318" s="11">
         <v>1</v>
       </c>
@@ -14879,7 +14878,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="319" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:14">
       <c r="A319" s="11">
         <v>1</v>
       </c>
@@ -14923,7 +14922,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="320" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:14">
       <c r="A320" s="11">
         <v>1</v>
       </c>
@@ -14967,7 +14966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="321" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:14">
       <c r="A321" s="11">
         <v>1</v>
       </c>
@@ -15011,7 +15010,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="322" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:14">
       <c r="A322" s="11">
         <v>1</v>
       </c>
@@ -15055,7 +15054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="323" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:14">
       <c r="A323" s="11">
         <v>1</v>
       </c>
@@ -15099,7 +15098,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="324" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:14">
       <c r="A324" s="11">
         <v>1</v>
       </c>
@@ -15143,7 +15142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="325" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:14">
       <c r="A325" s="11">
         <v>1</v>
       </c>
@@ -15187,7 +15186,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="326" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:14">
       <c r="A326" s="11">
         <v>1</v>
       </c>
@@ -15231,7 +15230,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="327" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:14">
       <c r="A327" s="11">
         <v>1</v>
       </c>
@@ -15275,7 +15274,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="328" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:14">
       <c r="A328" s="11">
         <v>1</v>
       </c>
@@ -15319,7 +15318,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="329" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:14">
       <c r="A329" s="11">
         <v>1</v>
       </c>
@@ -15363,7 +15362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="330" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:14">
       <c r="A330" s="11">
         <v>1</v>
       </c>
@@ -15407,7 +15406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="331" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:14">
       <c r="A331" s="11">
         <v>1</v>
       </c>
@@ -15451,7 +15450,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="332" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:14">
       <c r="A332" s="11">
         <v>1</v>
       </c>
@@ -15495,7 +15494,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="333" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:14">
       <c r="A333" s="11">
         <v>1</v>
       </c>
@@ -15539,7 +15538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="334" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:14">
       <c r="A334" s="11">
         <v>1</v>
       </c>
@@ -15583,7 +15582,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="335" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:14">
       <c r="A335" s="11">
         <v>1</v>
       </c>
@@ -15627,7 +15626,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="336" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:14">
       <c r="A336" s="11">
         <v>1</v>
       </c>
@@ -15671,7 +15670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="337" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:14">
       <c r="A337" s="11">
         <v>1</v>
       </c>
@@ -15715,7 +15714,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="338" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:14">
       <c r="A338" s="11">
         <v>1</v>
       </c>
@@ -15759,7 +15758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="339" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:14">
       <c r="A339" s="11">
         <v>1</v>
       </c>
@@ -15803,7 +15802,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="340" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:14">
       <c r="A340" s="11">
         <v>1</v>
       </c>
@@ -15847,7 +15846,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="341" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:14">
       <c r="A341" s="11">
         <v>1</v>
       </c>
@@ -15891,7 +15890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="342" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:14">
       <c r="A342" s="11">
         <v>1</v>
       </c>
@@ -15935,7 +15934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="343" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:14">
       <c r="A343" s="11">
         <v>1</v>
       </c>
@@ -15979,7 +15978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="344" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:14">
       <c r="A344" s="11">
         <v>1</v>
       </c>
@@ -16023,7 +16022,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="345" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:14">
       <c r="A345" s="11">
         <v>1</v>
       </c>
@@ -16067,7 +16066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="346" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:14">
       <c r="A346" s="11">
         <v>1</v>
       </c>
@@ -16111,7 +16110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="347" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:14">
       <c r="A347" s="11">
         <v>1</v>
       </c>
@@ -16155,7 +16154,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="348" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:14">
       <c r="A348" s="11">
         <v>1</v>
       </c>
@@ -16199,7 +16198,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="349" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:14">
       <c r="A349" s="11">
         <v>1</v>
       </c>
@@ -16243,7 +16242,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="350" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:14">
       <c r="A350" s="11">
         <v>1</v>
       </c>
@@ -16287,7 +16286,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="351" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:14">
       <c r="A351" s="11">
         <v>1</v>
       </c>
@@ -16331,7 +16330,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="352" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:14">
       <c r="A352" s="11">
         <v>1</v>
       </c>
@@ -16375,7 +16374,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="353" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:14">
       <c r="A353" s="11">
         <v>1</v>
       </c>
@@ -16419,7 +16418,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="354" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:14">
       <c r="A354" s="11">
         <v>1</v>
       </c>
@@ -16463,7 +16462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="355" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:14">
       <c r="A355" s="11">
         <v>1</v>
       </c>
@@ -16507,7 +16506,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="356" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:14">
       <c r="A356" s="11">
         <v>1</v>
       </c>
@@ -16551,7 +16550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="357" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:14">
       <c r="A357" s="11">
         <v>1</v>
       </c>
@@ -16595,7 +16594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="358" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:14">
       <c r="A358" s="11">
         <v>1</v>
       </c>
@@ -16639,7 +16638,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="359" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:14">
       <c r="A359" s="11">
         <v>1</v>
       </c>
@@ -16683,7 +16682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="360" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:14">
       <c r="A360" s="11">
         <v>1</v>
       </c>
@@ -16727,7 +16726,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="361" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:14">
       <c r="A361" s="11">
         <v>1</v>
       </c>
@@ -16771,7 +16770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="362" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:14">
       <c r="A362" s="11">
         <v>1</v>
       </c>
@@ -16815,7 +16814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="363" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:14">
       <c r="A363" s="11">
         <v>1</v>
       </c>
@@ -16859,7 +16858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="364" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:14">
       <c r="A364" s="11">
         <v>1</v>
       </c>
@@ -16903,7 +16902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="365" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:14">
       <c r="A365" s="11">
         <v>1</v>
       </c>
@@ -16947,7 +16946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="366" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:14">
       <c r="A366" s="11">
         <v>1</v>
       </c>
@@ -16991,7 +16990,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="367" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:14">
       <c r="A367" s="11">
         <v>1</v>
       </c>
@@ -17035,7 +17034,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="368" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:14">
       <c r="A368" s="11">
         <v>1</v>
       </c>
@@ -17079,7 +17078,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="369" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:14">
       <c r="A369" s="11">
         <v>1</v>
       </c>
@@ -17123,7 +17122,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="370" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:14">
       <c r="A370" s="11">
         <v>1</v>
       </c>
@@ -17167,7 +17166,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="371" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:14">
       <c r="A371" s="11">
         <v>1</v>
       </c>
@@ -17211,7 +17210,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="372" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:14">
       <c r="A372" s="11">
         <v>1</v>
       </c>
@@ -17255,7 +17254,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="373" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:14">
       <c r="A373" s="11">
         <v>1</v>
       </c>
@@ -17299,7 +17298,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="374" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:14">
       <c r="A374" s="11">
         <v>1</v>
       </c>
@@ -17343,7 +17342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="375" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:14">
       <c r="A375" s="11">
         <v>1</v>
       </c>
@@ -17387,7 +17386,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="376" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:14">
       <c r="A376" s="11">
         <v>1</v>
       </c>
@@ -17431,7 +17430,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="377" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:14">
       <c r="A377" s="11">
         <v>1</v>
       </c>
@@ -17475,7 +17474,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="378" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:14">
       <c r="A378" s="11">
         <v>1</v>
       </c>
@@ -17519,7 +17518,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="379" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:14">
       <c r="A379" s="11">
         <v>1</v>
       </c>
@@ -17563,7 +17562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="380" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:14">
       <c r="A380" s="11">
         <v>1</v>
       </c>
@@ -17607,7 +17606,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="381" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:14">
       <c r="A381" s="11">
         <v>1</v>
       </c>
@@ -17651,7 +17650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="382" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:14">
       <c r="A382" s="11">
         <v>1</v>
       </c>
@@ -17695,7 +17694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="383" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:14">
       <c r="A383" s="11">
         <v>1</v>
       </c>
@@ -17739,7 +17738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="384" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:14">
       <c r="A384" s="11">
         <v>1</v>
       </c>
@@ -17783,7 +17782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="385" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:14">
       <c r="A385" s="11">
         <v>1</v>
       </c>
@@ -17827,7 +17826,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="386" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:14">
       <c r="A386" s="11">
         <v>1</v>
       </c>
@@ -17871,7 +17870,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="387" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:14">
       <c r="A387" s="11">
         <v>1</v>
       </c>
@@ -17915,7 +17914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="388" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:14">
       <c r="A388" s="11">
         <v>1</v>
       </c>
@@ -17959,7 +17958,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="389" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:14">
       <c r="A389" s="11">
         <v>1</v>
       </c>
@@ -18003,7 +18002,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="390" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:14">
       <c r="A390" s="11">
         <v>1</v>
       </c>
@@ -18047,7 +18046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="391" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:14">
       <c r="A391" s="11">
         <v>1</v>
       </c>
@@ -18091,7 +18090,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="392" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:14">
       <c r="A392" s="11">
         <v>1</v>
       </c>
@@ -18135,7 +18134,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="393" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:14">
       <c r="A393" s="11">
         <v>1</v>
       </c>
@@ -18179,7 +18178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="394" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:14">
       <c r="A394" s="11">
         <v>1</v>
       </c>
@@ -18223,7 +18222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="395" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:14">
       <c r="A395" s="11">
         <v>1</v>
       </c>
@@ -18267,7 +18266,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="396" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:14">
       <c r="A396" s="11">
         <v>1</v>
       </c>
@@ -18311,7 +18310,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="397" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:14">
       <c r="A397" s="11">
         <v>1</v>
       </c>
@@ -18355,7 +18354,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="398" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:14">
       <c r="A398" s="11">
         <v>1</v>
       </c>
@@ -18399,7 +18398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="399" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:14">
       <c r="A399" s="11">
         <v>1</v>
       </c>
@@ -18443,7 +18442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="400" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:14">
       <c r="A400" s="11">
         <v>1</v>
       </c>
@@ -18487,7 +18486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="401" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:14">
       <c r="A401" s="11">
         <v>1</v>
       </c>
@@ -18531,7 +18530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="402" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:14">
       <c r="A402" s="12">
         <v>1</v>
       </c>
@@ -18585,26 +18584,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
-    <col min="7" max="7" width="30.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" customWidth="1"/>
     <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="9" max="9" width="30.5" customWidth="1"/>
-    <col min="10" max="10" width="30.83203125" customWidth="1"/>
-    <col min="11" max="11" width="34.6640625" customWidth="1"/>
-    <col min="12" max="12" width="31.5" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" customWidth="1"/>
+    <col min="11" max="11" width="34.7109375" customWidth="1"/>
+    <col min="12" max="12" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -18648,7 +18647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -18662,10 +18661,10 @@
         <v>9010101</v>
       </c>
       <c r="E2" s="11">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F2" s="11">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="G2" s="11">
         <v>0.6</v>
@@ -18702,27 +18701,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="7" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="7" width="20.42578125" customWidth="1"/>
     <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="9" max="9" width="30.5" customWidth="1"/>
-    <col min="10" max="10" width="30.83203125" customWidth="1"/>
-    <col min="11" max="11" width="34.6640625" customWidth="1"/>
-    <col min="12" max="12" width="31.5" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" customWidth="1"/>
+    <col min="11" max="11" width="34.7109375" customWidth="1"/>
+    <col min="12" max="12" width="31.42578125" customWidth="1"/>
     <col min="14" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18766,7 +18765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -18810,7 +18809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -18854,7 +18853,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -18898,7 +18897,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -18942,7 +18941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -18986,7 +18985,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -19030,7 +19029,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -19074,7 +19073,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -19118,7 +19117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -19162,7 +19161,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" s="4">
         <v>1</v>
       </c>
@@ -19206,7 +19205,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -19250,7 +19249,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="A13" s="4">
         <v>1</v>
       </c>
@@ -19294,7 +19293,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="A14" s="4">
         <v>1</v>
       </c>
@@ -19338,7 +19337,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="A15" s="4">
         <v>1</v>
       </c>
@@ -19382,7 +19381,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" s="4">
         <v>1</v>
       </c>
@@ -19426,7 +19425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14">
       <c r="A17" s="4">
         <v>1</v>
       </c>
@@ -19470,7 +19469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14">
       <c r="A18" s="4">
         <v>1</v>
       </c>
@@ -19514,7 +19513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14">
       <c r="A19" s="4">
         <v>1</v>
       </c>
@@ -19558,7 +19557,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14">
       <c r="A20" s="4">
         <v>1</v>
       </c>
@@ -19602,7 +19601,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14">
       <c r="A21" s="4">
         <v>1</v>
       </c>
@@ -19646,7 +19645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14">
       <c r="A22" s="4">
         <v>1</v>
       </c>
@@ -19690,7 +19689,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14">
       <c r="A23" s="4">
         <v>1</v>
       </c>
@@ -19734,7 +19733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14">
       <c r="A24" s="4">
         <v>1</v>
       </c>
@@ -19778,7 +19777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14">
       <c r="A25" s="4">
         <v>1</v>
       </c>
@@ -19822,7 +19821,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14">
       <c r="A26" s="4">
         <v>1</v>
       </c>
@@ -19866,7 +19865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14">
       <c r="A27" s="4">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
data collector bug fix
</commit_message>
<xml_diff>
--- a/projects/test_building/input/SimulatorScenarios.xlsx
+++ b/projects/test_building/input/SimulatorScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C043E495-E3E2-1644-9556-D403C5929E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4239B96-63B6-4A4C-97EC-D9D5BE12C2A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,46 +549,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:N402" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:N402" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:N402" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="start_year" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="end_year" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="id_region" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="building_num_min" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="building_num_max" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="name" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="comment" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="start_year" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="end_year" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="id_region" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="building_num_min" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="building_num_max" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="name" dataDxfId="17"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="comment" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:N2" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:N2" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A1:N2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="start_year" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="end_year" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_region" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="building_num_min" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="building_num_max" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="name" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="comment" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="start_year" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="end_year" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_region" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="building_num_min" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="building_num_max" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="name" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -882,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N402"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A333" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E337" sqref="E337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
energy_cost_before added and test_run folder files replaced with new results
</commit_message>
<xml_diff>
--- a/projects/test_building/input/SimulatorScenarios.xlsx
+++ b/projects/test_building/input/SimulatorScenarios.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yus\Documents\code\3E\RenderNew\projects\test_building\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844C7953-0BF5-8140-A3A0-AA5210C0213F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="765" windowWidth="16380" windowHeight="8205" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="2" r:id="rId1"/>
@@ -86,8 +85,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -613,75 +612,75 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:P2" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A1:P2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:P2" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A1:P2"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="start_year" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="end_year" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_region" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="building_num_min" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="building_num_max" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="22"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="renovation_mandatory" dataDxfId="21"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="heating_technology_mandatory" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="name" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="comment" dataDxfId="18"/>
+    <tableColumn id="1" name="id" dataDxfId="33"/>
+    <tableColumn id="2" name="start_year" dataDxfId="32"/>
+    <tableColumn id="3" name="end_year" dataDxfId="31"/>
+    <tableColumn id="4" name="id_region" dataDxfId="30"/>
+    <tableColumn id="5" name="building_num_min" dataDxfId="29"/>
+    <tableColumn id="6" name="building_num_max" dataDxfId="28"/>
+    <tableColumn id="7" name="optimal_heating_behavior_prob" dataDxfId="27"/>
+    <tableColumn id="8" name="id_scenario_energy_price_wholesale" dataDxfId="26"/>
+    <tableColumn id="9" name="id_scenario_energy_price_tax_rate" dataDxfId="25"/>
+    <tableColumn id="10" name="id_scenario_energy_price_mark_up" dataDxfId="24"/>
+    <tableColumn id="11" name="id_scenario_energy_price_co2_emission" dataDxfId="23"/>
+    <tableColumn id="12" name="id_scenario_energy_emission_factor" dataDxfId="22"/>
+    <tableColumn id="15" name="renovation_mandatory" dataDxfId="21"/>
+    <tableColumn id="16" name="heating_technology_mandatory" dataDxfId="20"/>
+    <tableColumn id="13" name="name" dataDxfId="19"/>
+    <tableColumn id="14" name="comment" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:P402" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:P402" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:P402" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:P402"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="start_year" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="end_year" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="id_region" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="building_num_min" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="building_num_max" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="renovation_mandatory" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="heating_technology_mandatory" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="name" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="comment" dataDxfId="0"/>
+    <tableColumn id="1" name="id" dataDxfId="15"/>
+    <tableColumn id="2" name="start_year" dataDxfId="14"/>
+    <tableColumn id="3" name="end_year" dataDxfId="13"/>
+    <tableColumn id="4" name="id_region" dataDxfId="12"/>
+    <tableColumn id="5" name="building_num_min" dataDxfId="11"/>
+    <tableColumn id="6" name="building_num_max" dataDxfId="10"/>
+    <tableColumn id="7" name="optimal_heating_behavior_prob" dataDxfId="9"/>
+    <tableColumn id="8" name="id_scenario_energy_price_wholesale" dataDxfId="8"/>
+    <tableColumn id="9" name="id_scenario_energy_price_tax_rate" dataDxfId="7"/>
+    <tableColumn id="10" name="id_scenario_energy_price_mark_up" dataDxfId="6"/>
+    <tableColumn id="11" name="id_scenario_energy_price_co2_emission" dataDxfId="5"/>
+    <tableColumn id="12" name="id_scenario_energy_emission_factor" dataDxfId="4"/>
+    <tableColumn id="15" name="renovation_mandatory" dataDxfId="3"/>
+    <tableColumn id="16" name="heating_technology_mandatory" dataDxfId="2"/>
+    <tableColumn id="13" name="name" dataDxfId="1"/>
+    <tableColumn id="14" name="comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:P27" totalsRowShown="0">
-  <autoFilter ref="A1:P27" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:P27" totalsRowShown="0">
+  <autoFilter ref="A1:P27"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="start_year"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="end_year"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="id_region"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="building_num_min"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="building_num_max"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="optimal_heating_behavior_prob"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="id_scenario_energy_price_wholesale"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="id_scenario_energy_price_tax_rate"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="id_scenario_energy_price_mark_up"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="id_scenario_energy_price_co2_emission"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="id_scenario_energy_emission_factor"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="renovation_mandatory"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="heating_technology_mandatory"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="name"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="comment"/>
+    <tableColumn id="1" name="id"/>
+    <tableColumn id="2" name="start_year"/>
+    <tableColumn id="3" name="end_year"/>
+    <tableColumn id="4" name="id_region"/>
+    <tableColumn id="5" name="building_num_min"/>
+    <tableColumn id="6" name="building_num_max"/>
+    <tableColumn id="7" name="optimal_heating_behavior_prob"/>
+    <tableColumn id="8" name="id_scenario_energy_price_wholesale"/>
+    <tableColumn id="9" name="id_scenario_energy_price_tax_rate"/>
+    <tableColumn id="10" name="id_scenario_energy_price_mark_up"/>
+    <tableColumn id="11" name="id_scenario_energy_price_co2_emission"/>
+    <tableColumn id="12" name="id_scenario_energy_emission_factor"/>
+    <tableColumn id="13" name="renovation_mandatory"/>
+    <tableColumn id="14" name="heating_technology_mandatory"/>
+    <tableColumn id="15" name="name"/>
+    <tableColumn id="16" name="comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -949,34 +948,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1026,7 +1025,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1040,10 +1039,10 @@
         <v>9010101</v>
       </c>
       <c r="E2" s="6">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F2" s="6">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="G2" s="6">
         <v>1</v>
@@ -1086,34 +1085,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P402"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1163,7 +1162,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1213,7 +1212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -1313,7 +1312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -1363,7 +1362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -1413,7 +1412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -1463,7 +1462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -1513,7 +1512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16">
       <c r="A9" s="6">
         <v>1</v>
       </c>
@@ -1563,7 +1562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16">
       <c r="A10" s="6">
         <v>1</v>
       </c>
@@ -1613,7 +1612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16">
       <c r="A11" s="6">
         <v>1</v>
       </c>
@@ -1663,7 +1662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16">
       <c r="A12" s="6">
         <v>1</v>
       </c>
@@ -1713,7 +1712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16">
       <c r="A13" s="6">
         <v>1</v>
       </c>
@@ -1763,7 +1762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16">
       <c r="A14" s="6">
         <v>1</v>
       </c>
@@ -1813,7 +1812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16">
       <c r="A15" s="6">
         <v>1</v>
       </c>
@@ -1863,7 +1862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16">
       <c r="A16" s="6">
         <v>1</v>
       </c>
@@ -1913,7 +1912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16">
       <c r="A17" s="6">
         <v>1</v>
       </c>
@@ -1963,7 +1962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16">
       <c r="A18" s="6">
         <v>1</v>
       </c>
@@ -2013,7 +2012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16">
       <c r="A19" s="6">
         <v>1</v>
       </c>
@@ -2063,7 +2062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16">
       <c r="A20" s="6">
         <v>1</v>
       </c>
@@ -2113,7 +2112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16">
       <c r="A21" s="6">
         <v>1</v>
       </c>
@@ -2163,7 +2162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16">
       <c r="A22" s="6">
         <v>1</v>
       </c>
@@ -2213,7 +2212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16">
       <c r="A23" s="6">
         <v>1</v>
       </c>
@@ -2263,7 +2262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16">
       <c r="A24" s="6">
         <v>1</v>
       </c>
@@ -2313,7 +2312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16">
       <c r="A25" s="6">
         <v>1</v>
       </c>
@@ -2363,7 +2362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16">
       <c r="A26" s="6">
         <v>1</v>
       </c>
@@ -2413,7 +2412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16">
       <c r="A27" s="6">
         <v>1</v>
       </c>
@@ -2463,7 +2462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16">
       <c r="A28" s="6">
         <v>1</v>
       </c>
@@ -2513,7 +2512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16">
       <c r="A29" s="6">
         <v>1</v>
       </c>
@@ -2563,7 +2562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16">
       <c r="A30" s="6">
         <v>1</v>
       </c>
@@ -2613,7 +2612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16">
       <c r="A31" s="6">
         <v>1</v>
       </c>
@@ -2663,7 +2662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16">
       <c r="A32" s="6">
         <v>1</v>
       </c>
@@ -2713,7 +2712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16">
       <c r="A33" s="6">
         <v>1</v>
       </c>
@@ -2763,7 +2762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16">
       <c r="A34" s="6">
         <v>1</v>
       </c>
@@ -2813,7 +2812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16">
       <c r="A35" s="6">
         <v>1</v>
       </c>
@@ -2863,7 +2862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16">
       <c r="A36" s="6">
         <v>1</v>
       </c>
@@ -2913,7 +2912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16">
       <c r="A37" s="6">
         <v>1</v>
       </c>
@@ -2963,7 +2962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16">
       <c r="A38" s="6">
         <v>1</v>
       </c>
@@ -3013,7 +3012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16">
       <c r="A39" s="6">
         <v>1</v>
       </c>
@@ -3063,7 +3062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16">
       <c r="A40" s="6">
         <v>1</v>
       </c>
@@ -3113,7 +3112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16">
       <c r="A41" s="6">
         <v>1</v>
       </c>
@@ -3163,7 +3162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16">
       <c r="A42" s="6">
         <v>1</v>
       </c>
@@ -3213,7 +3212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16">
       <c r="A43" s="6">
         <v>1</v>
       </c>
@@ -3263,7 +3262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16">
       <c r="A44" s="6">
         <v>1</v>
       </c>
@@ -3313,7 +3312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16">
       <c r="A45" s="6">
         <v>1</v>
       </c>
@@ -3363,7 +3362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16">
       <c r="A46" s="6">
         <v>1</v>
       </c>
@@ -3413,7 +3412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16">
       <c r="A47" s="6">
         <v>1</v>
       </c>
@@ -3463,7 +3462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16">
       <c r="A48" s="6">
         <v>1</v>
       </c>
@@ -3513,7 +3512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16">
       <c r="A49" s="6">
         <v>1</v>
       </c>
@@ -3563,7 +3562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16">
       <c r="A50" s="6">
         <v>1</v>
       </c>
@@ -3613,7 +3612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16">
       <c r="A51" s="6">
         <v>1</v>
       </c>
@@ -3663,7 +3662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16">
       <c r="A52" s="6">
         <v>1</v>
       </c>
@@ -3713,7 +3712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16">
       <c r="A53" s="6">
         <v>1</v>
       </c>
@@ -3763,7 +3762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16">
       <c r="A54" s="6">
         <v>1</v>
       </c>
@@ -3813,7 +3812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16">
       <c r="A55" s="6">
         <v>1</v>
       </c>
@@ -3863,7 +3862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16">
       <c r="A56" s="6">
         <v>1</v>
       </c>
@@ -3913,7 +3912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16">
       <c r="A57" s="6">
         <v>1</v>
       </c>
@@ -3963,7 +3962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16">
       <c r="A58" s="6">
         <v>1</v>
       </c>
@@ -4013,7 +4012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16">
       <c r="A59" s="6">
         <v>1</v>
       </c>
@@ -4063,7 +4062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16">
       <c r="A60" s="6">
         <v>1</v>
       </c>
@@ -4113,7 +4112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16">
       <c r="A61" s="6">
         <v>1</v>
       </c>
@@ -4163,7 +4162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16">
       <c r="A62" s="6">
         <v>1</v>
       </c>
@@ -4213,7 +4212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16">
       <c r="A63" s="6">
         <v>1</v>
       </c>
@@ -4263,7 +4262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16">
       <c r="A64" s="6">
         <v>1</v>
       </c>
@@ -4313,7 +4312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16">
       <c r="A65" s="6">
         <v>1</v>
       </c>
@@ -4363,7 +4362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16">
       <c r="A66" s="6">
         <v>1</v>
       </c>
@@ -4413,7 +4412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16">
       <c r="A67" s="6">
         <v>1</v>
       </c>
@@ -4463,7 +4462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16">
       <c r="A68" s="6">
         <v>1</v>
       </c>
@@ -4513,7 +4512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16">
       <c r="A69" s="6">
         <v>1</v>
       </c>
@@ -4563,7 +4562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16">
       <c r="A70" s="6">
         <v>1</v>
       </c>
@@ -4613,7 +4612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16">
       <c r="A71" s="6">
         <v>1</v>
       </c>
@@ -4663,7 +4662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16">
       <c r="A72" s="6">
         <v>1</v>
       </c>
@@ -4713,7 +4712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16">
       <c r="A73" s="6">
         <v>1</v>
       </c>
@@ -4763,7 +4762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16">
       <c r="A74" s="6">
         <v>1</v>
       </c>
@@ -4813,7 +4812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16">
       <c r="A75" s="6">
         <v>1</v>
       </c>
@@ -4863,7 +4862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16">
       <c r="A76" s="6">
         <v>1</v>
       </c>
@@ -4913,7 +4912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16">
       <c r="A77" s="6">
         <v>1</v>
       </c>
@@ -4963,7 +4962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16">
       <c r="A78" s="6">
         <v>1</v>
       </c>
@@ -5013,7 +5012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16">
       <c r="A79" s="6">
         <v>1</v>
       </c>
@@ -5063,7 +5062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16">
       <c r="A80" s="6">
         <v>1</v>
       </c>
@@ -5113,7 +5112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16">
       <c r="A81" s="6">
         <v>1</v>
       </c>
@@ -5163,7 +5162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16">
       <c r="A82" s="6">
         <v>1</v>
       </c>
@@ -5213,7 +5212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16">
       <c r="A83" s="6">
         <v>1</v>
       </c>
@@ -5263,7 +5262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16">
       <c r="A84" s="6">
         <v>1</v>
       </c>
@@ -5313,7 +5312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16">
       <c r="A85" s="6">
         <v>1</v>
       </c>
@@ -5363,7 +5362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16">
       <c r="A86" s="6">
         <v>1</v>
       </c>
@@ -5413,7 +5412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16">
       <c r="A87" s="6">
         <v>1</v>
       </c>
@@ -5463,7 +5462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16">
       <c r="A88" s="6">
         <v>1</v>
       </c>
@@ -5513,7 +5512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16">
       <c r="A89" s="6">
         <v>1</v>
       </c>
@@ -5563,7 +5562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16">
       <c r="A90" s="6">
         <v>1</v>
       </c>
@@ -5613,7 +5612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16">
       <c r="A91" s="6">
         <v>1</v>
       </c>
@@ -5663,7 +5662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16">
       <c r="A92" s="6">
         <v>1</v>
       </c>
@@ -5713,7 +5712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16">
       <c r="A93" s="6">
         <v>1</v>
       </c>
@@ -5763,7 +5762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16">
       <c r="A94" s="6">
         <v>1</v>
       </c>
@@ -5813,7 +5812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16">
       <c r="A95" s="6">
         <v>1</v>
       </c>
@@ -5863,7 +5862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16">
       <c r="A96" s="6">
         <v>1</v>
       </c>
@@ -5913,7 +5912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16">
       <c r="A97" s="6">
         <v>1</v>
       </c>
@@ -5963,7 +5962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16">
       <c r="A98" s="6">
         <v>1</v>
       </c>
@@ -6013,7 +6012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16">
       <c r="A99" s="6">
         <v>1</v>
       </c>
@@ -6063,7 +6062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16">
       <c r="A100" s="6">
         <v>1</v>
       </c>
@@ -6113,7 +6112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16">
       <c r="A101" s="6">
         <v>1</v>
       </c>
@@ -6163,7 +6162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16">
       <c r="A102" s="6">
         <v>1</v>
       </c>
@@ -6213,7 +6212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16">
       <c r="A103" s="6">
         <v>1</v>
       </c>
@@ -6263,7 +6262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16">
       <c r="A104" s="6">
         <v>1</v>
       </c>
@@ -6313,7 +6312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16">
       <c r="A105" s="6">
         <v>1</v>
       </c>
@@ -6363,7 +6362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16">
       <c r="A106" s="6">
         <v>1</v>
       </c>
@@ -6413,7 +6412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16">
       <c r="A107" s="6">
         <v>1</v>
       </c>
@@ -6463,7 +6462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16">
       <c r="A108" s="6">
         <v>1</v>
       </c>
@@ -6513,7 +6512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16">
       <c r="A109" s="6">
         <v>1</v>
       </c>
@@ -6563,7 +6562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16">
       <c r="A110" s="6">
         <v>1</v>
       </c>
@@ -6613,7 +6612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16">
       <c r="A111" s="6">
         <v>1</v>
       </c>
@@ -6663,7 +6662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:16">
       <c r="A112" s="6">
         <v>1</v>
       </c>
@@ -6713,7 +6712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16">
       <c r="A113" s="6">
         <v>1</v>
       </c>
@@ -6763,7 +6762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16">
       <c r="A114" s="6">
         <v>1</v>
       </c>
@@ -6813,7 +6812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16">
       <c r="A115" s="6">
         <v>1</v>
       </c>
@@ -6863,7 +6862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16">
       <c r="A116" s="6">
         <v>1</v>
       </c>
@@ -6913,7 +6912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16">
       <c r="A117" s="6">
         <v>1</v>
       </c>
@@ -6963,7 +6962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16">
       <c r="A118" s="6">
         <v>1</v>
       </c>
@@ -7013,7 +7012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16">
       <c r="A119" s="6">
         <v>1</v>
       </c>
@@ -7063,7 +7062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16">
       <c r="A120" s="6">
         <v>1</v>
       </c>
@@ -7113,7 +7112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16">
       <c r="A121" s="6">
         <v>1</v>
       </c>
@@ -7163,7 +7162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16">
       <c r="A122" s="6">
         <v>1</v>
       </c>
@@ -7213,7 +7212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16">
       <c r="A123" s="6">
         <v>1</v>
       </c>
@@ -7263,7 +7262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16">
       <c r="A124" s="6">
         <v>1</v>
       </c>
@@ -7313,7 +7312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16">
       <c r="A125" s="6">
         <v>1</v>
       </c>
@@ -7363,7 +7362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16">
       <c r="A126" s="6">
         <v>1</v>
       </c>
@@ -7413,7 +7412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16">
       <c r="A127" s="6">
         <v>1</v>
       </c>
@@ -7463,7 +7462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16">
       <c r="A128" s="6">
         <v>1</v>
       </c>
@@ -7513,7 +7512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16">
       <c r="A129" s="6">
         <v>1</v>
       </c>
@@ -7563,7 +7562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16">
       <c r="A130" s="6">
         <v>1</v>
       </c>
@@ -7613,7 +7612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16">
       <c r="A131" s="6">
         <v>1</v>
       </c>
@@ -7663,7 +7662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16">
       <c r="A132" s="6">
         <v>1</v>
       </c>
@@ -7713,7 +7712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16">
       <c r="A133" s="6">
         <v>1</v>
       </c>
@@ -7763,7 +7762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16">
       <c r="A134" s="6">
         <v>1</v>
       </c>
@@ -7813,7 +7812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16">
       <c r="A135" s="6">
         <v>1</v>
       </c>
@@ -7863,7 +7862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16">
       <c r="A136" s="6">
         <v>1</v>
       </c>
@@ -7913,7 +7912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16">
       <c r="A137" s="6">
         <v>1</v>
       </c>
@@ -7963,7 +7962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16">
       <c r="A138" s="6">
         <v>1</v>
       </c>
@@ -8013,7 +8012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16">
       <c r="A139" s="6">
         <v>1</v>
       </c>
@@ -8063,7 +8062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16">
       <c r="A140" s="6">
         <v>1</v>
       </c>
@@ -8113,7 +8112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16">
       <c r="A141" s="6">
         <v>1</v>
       </c>
@@ -8163,7 +8162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16">
       <c r="A142" s="6">
         <v>1</v>
       </c>
@@ -8213,7 +8212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16">
       <c r="A143" s="6">
         <v>1</v>
       </c>
@@ -8263,7 +8262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16">
       <c r="A144" s="6">
         <v>1</v>
       </c>
@@ -8313,7 +8312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16">
       <c r="A145" s="6">
         <v>1</v>
       </c>
@@ -8363,7 +8362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16">
       <c r="A146" s="6">
         <v>1</v>
       </c>
@@ -8413,7 +8412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16">
       <c r="A147" s="6">
         <v>1</v>
       </c>
@@ -8463,7 +8462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16">
       <c r="A148" s="6">
         <v>1</v>
       </c>
@@ -8513,7 +8512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16">
       <c r="A149" s="6">
         <v>1</v>
       </c>
@@ -8563,7 +8562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16">
       <c r="A150" s="6">
         <v>1</v>
       </c>
@@ -8613,7 +8612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16">
       <c r="A151" s="6">
         <v>1</v>
       </c>
@@ -8663,7 +8662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16">
       <c r="A152" s="6">
         <v>1</v>
       </c>
@@ -8713,7 +8712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16">
       <c r="A153" s="6">
         <v>1</v>
       </c>
@@ -8763,7 +8762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16">
       <c r="A154" s="6">
         <v>1</v>
       </c>
@@ -8813,7 +8812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:16">
       <c r="A155" s="6">
         <v>1</v>
       </c>
@@ -8863,7 +8862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:16">
       <c r="A156" s="6">
         <v>1</v>
       </c>
@@ -8913,7 +8912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:16">
       <c r="A157" s="6">
         <v>1</v>
       </c>
@@ -8963,7 +8962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:16">
       <c r="A158" s="6">
         <v>1</v>
       </c>
@@ -9013,7 +9012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:16">
       <c r="A159" s="6">
         <v>1</v>
       </c>
@@ -9063,7 +9062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:16">
       <c r="A160" s="6">
         <v>1</v>
       </c>
@@ -9113,7 +9112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:16">
       <c r="A161" s="6">
         <v>1</v>
       </c>
@@ -9163,7 +9162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16">
       <c r="A162" s="6">
         <v>1</v>
       </c>
@@ -9213,7 +9212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16">
       <c r="A163" s="6">
         <v>1</v>
       </c>
@@ -9263,7 +9262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16">
       <c r="A164" s="6">
         <v>1</v>
       </c>
@@ -9313,7 +9312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16">
       <c r="A165" s="6">
         <v>1</v>
       </c>
@@ -9363,7 +9362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16">
       <c r="A166" s="6">
         <v>1</v>
       </c>
@@ -9413,7 +9412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16">
       <c r="A167" s="6">
         <v>1</v>
       </c>
@@ -9463,7 +9462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16">
       <c r="A168" s="6">
         <v>1</v>
       </c>
@@ -9513,7 +9512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16">
       <c r="A169" s="6">
         <v>1</v>
       </c>
@@ -9563,7 +9562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16">
       <c r="A170" s="6">
         <v>1</v>
       </c>
@@ -9613,7 +9612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16">
       <c r="A171" s="6">
         <v>1</v>
       </c>
@@ -9663,7 +9662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16">
       <c r="A172" s="6">
         <v>1</v>
       </c>
@@ -9713,7 +9712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:16">
       <c r="A173" s="6">
         <v>1</v>
       </c>
@@ -9763,7 +9762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:16">
       <c r="A174" s="6">
         <v>1</v>
       </c>
@@ -9813,7 +9812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:16">
       <c r="A175" s="6">
         <v>1</v>
       </c>
@@ -9863,7 +9862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:16">
       <c r="A176" s="6">
         <v>1</v>
       </c>
@@ -9913,7 +9912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:16">
       <c r="A177" s="6">
         <v>1</v>
       </c>
@@ -9963,7 +9962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:16">
       <c r="A178" s="6">
         <v>1</v>
       </c>
@@ -10013,7 +10012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:16">
       <c r="A179" s="6">
         <v>1</v>
       </c>
@@ -10063,7 +10062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:16">
       <c r="A180" s="6">
         <v>1</v>
       </c>
@@ -10113,7 +10112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:16">
       <c r="A181" s="6">
         <v>1</v>
       </c>
@@ -10163,7 +10162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:16">
       <c r="A182" s="6">
         <v>1</v>
       </c>
@@ -10213,7 +10212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:16">
       <c r="A183" s="6">
         <v>1</v>
       </c>
@@ -10263,7 +10262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:16">
       <c r="A184" s="6">
         <v>1</v>
       </c>
@@ -10313,7 +10312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:16">
       <c r="A185" s="6">
         <v>1</v>
       </c>
@@ -10363,7 +10362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:16">
       <c r="A186" s="6">
         <v>1</v>
       </c>
@@ -10413,7 +10412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:16">
       <c r="A187" s="6">
         <v>1</v>
       </c>
@@ -10463,7 +10462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:16">
       <c r="A188" s="6">
         <v>1</v>
       </c>
@@ -10513,7 +10512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:16">
       <c r="A189" s="6">
         <v>1</v>
       </c>
@@ -10563,7 +10562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:16">
       <c r="A190" s="6">
         <v>1</v>
       </c>
@@ -10613,7 +10612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:16">
       <c r="A191" s="6">
         <v>1</v>
       </c>
@@ -10663,7 +10662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:16">
       <c r="A192" s="6">
         <v>1</v>
       </c>
@@ -10713,7 +10712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:16">
       <c r="A193" s="6">
         <v>1</v>
       </c>
@@ -10763,7 +10762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:16">
       <c r="A194" s="6">
         <v>1</v>
       </c>
@@ -10813,7 +10812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:16">
       <c r="A195" s="6">
         <v>1</v>
       </c>
@@ -10863,7 +10862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:16">
       <c r="A196" s="6">
         <v>1</v>
       </c>
@@ -10913,7 +10912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:16">
       <c r="A197" s="6">
         <v>1</v>
       </c>
@@ -10963,7 +10962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:16">
       <c r="A198" s="6">
         <v>1</v>
       </c>
@@ -11013,7 +11012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:16">
       <c r="A199" s="6">
         <v>1</v>
       </c>
@@ -11063,7 +11062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:16">
       <c r="A200" s="6">
         <v>1</v>
       </c>
@@ -11113,7 +11112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:16">
       <c r="A201" s="6">
         <v>1</v>
       </c>
@@ -11163,7 +11162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:16">
       <c r="A202" s="6">
         <v>1</v>
       </c>
@@ -11213,7 +11212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:16">
       <c r="A203" s="6">
         <v>1</v>
       </c>
@@ -11263,7 +11262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:16">
       <c r="A204" s="6">
         <v>1</v>
       </c>
@@ -11313,7 +11312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:16">
       <c r="A205" s="6">
         <v>1</v>
       </c>
@@ -11363,7 +11362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:16">
       <c r="A206" s="6">
         <v>1</v>
       </c>
@@ -11413,7 +11412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:16">
       <c r="A207" s="6">
         <v>1</v>
       </c>
@@ -11463,7 +11462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:16">
       <c r="A208" s="6">
         <v>1</v>
       </c>
@@ -11513,7 +11512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:16">
       <c r="A209" s="6">
         <v>1</v>
       </c>
@@ -11563,7 +11562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:16">
       <c r="A210" s="6">
         <v>1</v>
       </c>
@@ -11613,7 +11612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:16">
       <c r="A211" s="6">
         <v>1</v>
       </c>
@@ -11663,7 +11662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:16">
       <c r="A212" s="6">
         <v>1</v>
       </c>
@@ -11713,7 +11712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:16">
       <c r="A213" s="6">
         <v>1</v>
       </c>
@@ -11763,7 +11762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:16">
       <c r="A214" s="6">
         <v>1</v>
       </c>
@@ -11813,7 +11812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:16">
       <c r="A215" s="6">
         <v>1</v>
       </c>
@@ -11863,7 +11862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:16">
       <c r="A216" s="6">
         <v>1</v>
       </c>
@@ -11913,7 +11912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:16">
       <c r="A217" s="6">
         <v>1</v>
       </c>
@@ -11963,7 +11962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:16">
       <c r="A218" s="6">
         <v>1</v>
       </c>
@@ -12013,7 +12012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:16">
       <c r="A219" s="6">
         <v>1</v>
       </c>
@@ -12063,7 +12062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:16">
       <c r="A220" s="6">
         <v>1</v>
       </c>
@@ -12113,7 +12112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:16">
       <c r="A221" s="6">
         <v>1</v>
       </c>
@@ -12163,7 +12162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:16">
       <c r="A222" s="6">
         <v>1</v>
       </c>
@@ -12213,7 +12212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:16">
       <c r="A223" s="6">
         <v>1</v>
       </c>
@@ -12263,7 +12262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:16">
       <c r="A224" s="6">
         <v>1</v>
       </c>
@@ -12313,7 +12312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:16">
       <c r="A225" s="6">
         <v>1</v>
       </c>
@@ -12363,7 +12362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="226" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:16">
       <c r="A226" s="6">
         <v>1</v>
       </c>
@@ -12413,7 +12412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:16">
       <c r="A227" s="6">
         <v>1</v>
       </c>
@@ -12463,7 +12462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="228" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:16">
       <c r="A228" s="6">
         <v>1</v>
       </c>
@@ -12513,7 +12512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="229" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:16">
       <c r="A229" s="6">
         <v>1</v>
       </c>
@@ -12563,7 +12562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:16">
       <c r="A230" s="6">
         <v>1</v>
       </c>
@@ -12613,7 +12612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="231" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:16">
       <c r="A231" s="6">
         <v>1</v>
       </c>
@@ -12663,7 +12662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="232" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:16">
       <c r="A232" s="6">
         <v>1</v>
       </c>
@@ -12713,7 +12712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:16">
       <c r="A233" s="6">
         <v>1</v>
       </c>
@@ -12763,7 +12762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:16">
       <c r="A234" s="6">
         <v>1</v>
       </c>
@@ -12813,7 +12812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:16">
       <c r="A235" s="6">
         <v>1</v>
       </c>
@@ -12863,7 +12862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:16">
       <c r="A236" s="6">
         <v>1</v>
       </c>
@@ -12913,7 +12912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:16">
       <c r="A237" s="6">
         <v>1</v>
       </c>
@@ -12963,7 +12962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="238" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:16">
       <c r="A238" s="6">
         <v>1</v>
       </c>
@@ -13013,7 +13012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:16">
       <c r="A239" s="6">
         <v>1</v>
       </c>
@@ -13063,7 +13062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:16">
       <c r="A240" s="6">
         <v>1</v>
       </c>
@@ -13113,7 +13112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:16">
       <c r="A241" s="6">
         <v>1</v>
       </c>
@@ -13163,7 +13162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:16">
       <c r="A242" s="6">
         <v>1</v>
       </c>
@@ -13213,7 +13212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="243" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:16">
       <c r="A243" s="6">
         <v>1</v>
       </c>
@@ -13263,7 +13262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="244" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:16">
       <c r="A244" s="6">
         <v>1</v>
       </c>
@@ -13313,7 +13312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:16">
       <c r="A245" s="6">
         <v>1</v>
       </c>
@@ -13363,7 +13362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="246" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:16">
       <c r="A246" s="6">
         <v>1</v>
       </c>
@@ -13413,7 +13412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="247" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:16">
       <c r="A247" s="6">
         <v>1</v>
       </c>
@@ -13463,7 +13462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:16">
       <c r="A248" s="6">
         <v>1</v>
       </c>
@@ -13513,7 +13512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:16">
       <c r="A249" s="6">
         <v>1</v>
       </c>
@@ -13563,7 +13562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="250" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:16">
       <c r="A250" s="6">
         <v>1</v>
       </c>
@@ -13613,7 +13612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:16">
       <c r="A251" s="6">
         <v>1</v>
       </c>
@@ -13663,7 +13662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="252" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:16">
       <c r="A252" s="6">
         <v>1</v>
       </c>
@@ -13713,7 +13712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="253" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:16">
       <c r="A253" s="6">
         <v>1</v>
       </c>
@@ -13763,7 +13762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="254" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:16">
       <c r="A254" s="6">
         <v>1</v>
       </c>
@@ -13813,7 +13812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="255" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:16">
       <c r="A255" s="6">
         <v>1</v>
       </c>
@@ -13863,7 +13862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="256" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:16">
       <c r="A256" s="6">
         <v>1</v>
       </c>
@@ -13913,7 +13912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="257" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:16">
       <c r="A257" s="6">
         <v>1</v>
       </c>
@@ -13963,7 +13962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="258" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:16">
       <c r="A258" s="6">
         <v>1</v>
       </c>
@@ -14013,7 +14012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="259" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:16">
       <c r="A259" s="6">
         <v>1</v>
       </c>
@@ -14063,7 +14062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="260" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:16">
       <c r="A260" s="6">
         <v>1</v>
       </c>
@@ -14113,7 +14112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="261" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:16">
       <c r="A261" s="6">
         <v>1</v>
       </c>
@@ -14163,7 +14162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:16">
       <c r="A262" s="6">
         <v>1</v>
       </c>
@@ -14213,7 +14212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="263" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:16">
       <c r="A263" s="6">
         <v>1</v>
       </c>
@@ -14263,7 +14262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:16">
       <c r="A264" s="6">
         <v>1</v>
       </c>
@@ -14313,7 +14312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="265" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:16">
       <c r="A265" s="6">
         <v>1</v>
       </c>
@@ -14363,7 +14362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="266" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:16">
       <c r="A266" s="6">
         <v>1</v>
       </c>
@@ -14413,7 +14412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="267" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:16">
       <c r="A267" s="6">
         <v>1</v>
       </c>
@@ -14463,7 +14462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="268" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:16">
       <c r="A268" s="6">
         <v>1</v>
       </c>
@@ -14513,7 +14512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="269" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:16">
       <c r="A269" s="6">
         <v>1</v>
       </c>
@@ -14563,7 +14562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="270" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:16">
       <c r="A270" s="6">
         <v>1</v>
       </c>
@@ -14613,7 +14612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="271" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:16">
       <c r="A271" s="6">
         <v>1</v>
       </c>
@@ -14663,7 +14662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="272" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:16">
       <c r="A272" s="6">
         <v>1</v>
       </c>
@@ -14713,7 +14712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="273" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:16">
       <c r="A273" s="6">
         <v>1</v>
       </c>
@@ -14763,7 +14762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="274" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:16">
       <c r="A274" s="6">
         <v>1</v>
       </c>
@@ -14813,7 +14812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="275" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:16">
       <c r="A275" s="6">
         <v>1</v>
       </c>
@@ -14863,7 +14862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="276" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:16">
       <c r="A276" s="6">
         <v>1</v>
       </c>
@@ -14913,7 +14912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="277" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:16">
       <c r="A277" s="6">
         <v>1</v>
       </c>
@@ -14963,7 +14962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="278" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:16">
       <c r="A278" s="6">
         <v>1</v>
       </c>
@@ -15013,7 +15012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="279" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:16">
       <c r="A279" s="6">
         <v>1</v>
       </c>
@@ -15063,7 +15062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="280" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:16">
       <c r="A280" s="6">
         <v>1</v>
       </c>
@@ -15113,7 +15112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="281" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:16">
       <c r="A281" s="6">
         <v>1</v>
       </c>
@@ -15163,7 +15162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="282" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:16">
       <c r="A282" s="6">
         <v>1</v>
       </c>
@@ -15213,7 +15212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="283" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:16">
       <c r="A283" s="6">
         <v>1</v>
       </c>
@@ -15263,7 +15262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="284" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:16">
       <c r="A284" s="6">
         <v>1</v>
       </c>
@@ -15313,7 +15312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="285" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:16">
       <c r="A285" s="6">
         <v>1</v>
       </c>
@@ -15363,7 +15362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="286" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:16">
       <c r="A286" s="6">
         <v>1</v>
       </c>
@@ -15413,7 +15412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="287" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:16">
       <c r="A287" s="6">
         <v>1</v>
       </c>
@@ -15463,7 +15462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="288" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:16">
       <c r="A288" s="6">
         <v>1</v>
       </c>
@@ -15513,7 +15512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:16">
       <c r="A289" s="6">
         <v>1</v>
       </c>
@@ -15563,7 +15562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:16">
       <c r="A290" s="6">
         <v>1</v>
       </c>
@@ -15613,7 +15612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="291" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:16">
       <c r="A291" s="6">
         <v>1</v>
       </c>
@@ -15663,7 +15662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:16">
       <c r="A292" s="6">
         <v>1</v>
       </c>
@@ -15713,7 +15712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="293" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:16">
       <c r="A293" s="6">
         <v>1</v>
       </c>
@@ -15763,7 +15762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="294" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:16">
       <c r="A294" s="6">
         <v>1</v>
       </c>
@@ -15813,7 +15812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:16">
       <c r="A295" s="6">
         <v>1</v>
       </c>
@@ -15863,7 +15862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:16">
       <c r="A296" s="6">
         <v>1</v>
       </c>
@@ -15913,7 +15912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="297" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:16">
       <c r="A297" s="6">
         <v>1</v>
       </c>
@@ -15963,7 +15962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="298" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:16">
       <c r="A298" s="6">
         <v>1</v>
       </c>
@@ -16013,7 +16012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="299" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:16">
       <c r="A299" s="6">
         <v>1</v>
       </c>
@@ -16063,7 +16062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="300" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:16">
       <c r="A300" s="6">
         <v>1</v>
       </c>
@@ -16113,7 +16112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="301" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:16">
       <c r="A301" s="6">
         <v>1</v>
       </c>
@@ -16163,7 +16162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="302" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:16">
       <c r="A302" s="6">
         <v>1</v>
       </c>
@@ -16213,7 +16212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="303" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:16">
       <c r="A303" s="6">
         <v>1</v>
       </c>
@@ -16263,7 +16262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="304" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:16">
       <c r="A304" s="6">
         <v>1</v>
       </c>
@@ -16313,7 +16312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="305" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:16">
       <c r="A305" s="6">
         <v>1</v>
       </c>
@@ -16363,7 +16362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="306" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:16">
       <c r="A306" s="6">
         <v>1</v>
       </c>
@@ -16413,7 +16412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="307" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:16">
       <c r="A307" s="6">
         <v>1</v>
       </c>
@@ -16463,7 +16462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="308" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:16">
       <c r="A308" s="6">
         <v>1</v>
       </c>
@@ -16513,7 +16512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:16">
       <c r="A309" s="6">
         <v>1</v>
       </c>
@@ -16563,7 +16562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="310" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:16">
       <c r="A310" s="6">
         <v>1</v>
       </c>
@@ -16613,7 +16612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="311" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:16">
       <c r="A311" s="6">
         <v>1</v>
       </c>
@@ -16663,7 +16662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="312" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:16">
       <c r="A312" s="6">
         <v>1</v>
       </c>
@@ -16713,7 +16712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="313" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:16">
       <c r="A313" s="6">
         <v>1</v>
       </c>
@@ -16763,7 +16762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="314" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:16">
       <c r="A314" s="6">
         <v>1</v>
       </c>
@@ -16813,7 +16812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="315" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:16">
       <c r="A315" s="6">
         <v>1</v>
       </c>
@@ -16863,7 +16862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="316" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:16">
       <c r="A316" s="6">
         <v>1</v>
       </c>
@@ -16913,7 +16912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="317" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:16">
       <c r="A317" s="6">
         <v>1</v>
       </c>
@@ -16963,7 +16962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="318" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:16">
       <c r="A318" s="6">
         <v>1</v>
       </c>
@@ -17013,7 +17012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="319" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:16">
       <c r="A319" s="6">
         <v>1</v>
       </c>
@@ -17063,7 +17062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="320" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:16">
       <c r="A320" s="6">
         <v>1</v>
       </c>
@@ -17113,7 +17112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="321" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:16">
       <c r="A321" s="6">
         <v>1</v>
       </c>
@@ -17163,7 +17162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="322" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:16">
       <c r="A322" s="6">
         <v>1</v>
       </c>
@@ -17213,7 +17212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="323" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:16">
       <c r="A323" s="6">
         <v>1</v>
       </c>
@@ -17263,7 +17262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="324" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:16">
       <c r="A324" s="6">
         <v>1</v>
       </c>
@@ -17313,7 +17312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="325" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:16">
       <c r="A325" s="6">
         <v>1</v>
       </c>
@@ -17363,7 +17362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="326" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:16">
       <c r="A326" s="6">
         <v>1</v>
       </c>
@@ -17413,7 +17412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="327" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:16">
       <c r="A327" s="6">
         <v>1</v>
       </c>
@@ -17463,7 +17462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="328" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:16">
       <c r="A328" s="6">
         <v>1</v>
       </c>
@@ -17513,7 +17512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="329" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:16">
       <c r="A329" s="6">
         <v>1</v>
       </c>
@@ -17563,7 +17562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="330" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:16">
       <c r="A330" s="6">
         <v>1</v>
       </c>
@@ -17613,7 +17612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="331" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:16">
       <c r="A331" s="6">
         <v>1</v>
       </c>
@@ -17663,7 +17662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="332" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:16">
       <c r="A332" s="6">
         <v>1</v>
       </c>
@@ -17713,7 +17712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="333" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:16">
       <c r="A333" s="6">
         <v>1</v>
       </c>
@@ -17763,7 +17762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="334" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:16">
       <c r="A334" s="6">
         <v>1</v>
       </c>
@@ -17813,7 +17812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="335" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:16">
       <c r="A335" s="6">
         <v>1</v>
       </c>
@@ -17863,7 +17862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="336" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:16">
       <c r="A336" s="6">
         <v>1</v>
       </c>
@@ -17913,7 +17912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="337" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:16">
       <c r="A337" s="6">
         <v>1</v>
       </c>
@@ -17963,7 +17962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="338" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:16">
       <c r="A338" s="6">
         <v>1</v>
       </c>
@@ -18013,7 +18012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="339" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:16">
       <c r="A339" s="6">
         <v>1</v>
       </c>
@@ -18063,7 +18062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="340" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:16">
       <c r="A340" s="6">
         <v>1</v>
       </c>
@@ -18113,7 +18112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="341" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:16">
       <c r="A341" s="6">
         <v>1</v>
       </c>
@@ -18163,7 +18162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="342" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:16">
       <c r="A342" s="6">
         <v>1</v>
       </c>
@@ -18213,7 +18212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="343" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:16">
       <c r="A343" s="6">
         <v>1</v>
       </c>
@@ -18263,7 +18262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="344" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:16">
       <c r="A344" s="6">
         <v>1</v>
       </c>
@@ -18313,7 +18312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="345" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:16">
       <c r="A345" s="6">
         <v>1</v>
       </c>
@@ -18363,7 +18362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="346" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:16">
       <c r="A346" s="6">
         <v>1</v>
       </c>
@@ -18413,7 +18412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="347" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:16">
       <c r="A347" s="6">
         <v>1</v>
       </c>
@@ -18463,7 +18462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="348" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:16">
       <c r="A348" s="6">
         <v>1</v>
       </c>
@@ -18513,7 +18512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="349" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:16">
       <c r="A349" s="6">
         <v>1</v>
       </c>
@@ -18563,7 +18562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="350" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:16">
       <c r="A350" s="6">
         <v>1</v>
       </c>
@@ -18613,7 +18612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="351" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:16">
       <c r="A351" s="6">
         <v>1</v>
       </c>
@@ -18663,7 +18662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="352" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:16">
       <c r="A352" s="6">
         <v>1</v>
       </c>
@@ -18713,7 +18712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="353" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:16">
       <c r="A353" s="6">
         <v>1</v>
       </c>
@@ -18763,7 +18762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="354" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:16">
       <c r="A354" s="6">
         <v>1</v>
       </c>
@@ -18813,7 +18812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="355" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:16">
       <c r="A355" s="6">
         <v>1</v>
       </c>
@@ -18863,7 +18862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="356" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:16">
       <c r="A356" s="6">
         <v>1</v>
       </c>
@@ -18913,7 +18912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="357" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:16">
       <c r="A357" s="6">
         <v>1</v>
       </c>
@@ -18963,7 +18962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="358" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:16">
       <c r="A358" s="6">
         <v>1</v>
       </c>
@@ -19013,7 +19012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="359" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:16">
       <c r="A359" s="6">
         <v>1</v>
       </c>
@@ -19063,7 +19062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="360" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:16">
       <c r="A360" s="6">
         <v>1</v>
       </c>
@@ -19113,7 +19112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="361" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:16">
       <c r="A361" s="6">
         <v>1</v>
       </c>
@@ -19163,7 +19162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="362" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:16">
       <c r="A362" s="6">
         <v>1</v>
       </c>
@@ -19213,7 +19212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="363" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:16">
       <c r="A363" s="6">
         <v>1</v>
       </c>
@@ -19263,7 +19262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="364" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:16">
       <c r="A364" s="6">
         <v>1</v>
       </c>
@@ -19313,7 +19312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="365" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:16">
       <c r="A365" s="6">
         <v>1</v>
       </c>
@@ -19363,7 +19362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="366" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:16">
       <c r="A366" s="6">
         <v>1</v>
       </c>
@@ -19413,7 +19412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="367" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:16">
       <c r="A367" s="6">
         <v>1</v>
       </c>
@@ -19463,7 +19462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="368" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:16">
       <c r="A368" s="6">
         <v>1</v>
       </c>
@@ -19513,7 +19512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="369" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:16">
       <c r="A369" s="6">
         <v>1</v>
       </c>
@@ -19563,7 +19562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="370" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:16">
       <c r="A370" s="6">
         <v>1</v>
       </c>
@@ -19613,7 +19612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="371" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:16">
       <c r="A371" s="6">
         <v>1</v>
       </c>
@@ -19663,7 +19662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="372" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:16">
       <c r="A372" s="6">
         <v>1</v>
       </c>
@@ -19713,7 +19712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="373" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:16">
       <c r="A373" s="6">
         <v>1</v>
       </c>
@@ -19763,7 +19762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="374" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:16">
       <c r="A374" s="6">
         <v>1</v>
       </c>
@@ -19813,7 +19812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="375" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:16">
       <c r="A375" s="6">
         <v>1</v>
       </c>
@@ -19863,7 +19862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="376" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:16">
       <c r="A376" s="6">
         <v>1</v>
       </c>
@@ -19913,7 +19912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="377" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:16">
       <c r="A377" s="6">
         <v>1</v>
       </c>
@@ -19963,7 +19962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="378" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:16">
       <c r="A378" s="6">
         <v>1</v>
       </c>
@@ -20013,7 +20012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="379" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:16">
       <c r="A379" s="6">
         <v>1</v>
       </c>
@@ -20063,7 +20062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="380" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:16">
       <c r="A380" s="6">
         <v>1</v>
       </c>
@@ -20113,7 +20112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="381" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:16">
       <c r="A381" s="6">
         <v>1</v>
       </c>
@@ -20163,7 +20162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="382" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:16">
       <c r="A382" s="6">
         <v>1</v>
       </c>
@@ -20213,7 +20212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="383" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:16">
       <c r="A383" s="6">
         <v>1</v>
       </c>
@@ -20263,7 +20262,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="384" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:16">
       <c r="A384" s="6">
         <v>1</v>
       </c>
@@ -20313,7 +20312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="385" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:16">
       <c r="A385" s="6">
         <v>1</v>
       </c>
@@ -20363,7 +20362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="386" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:16">
       <c r="A386" s="6">
         <v>1</v>
       </c>
@@ -20413,7 +20412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="387" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:16">
       <c r="A387" s="6">
         <v>1</v>
       </c>
@@ -20463,7 +20462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="388" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:16">
       <c r="A388" s="6">
         <v>1</v>
       </c>
@@ -20513,7 +20512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="389" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:16">
       <c r="A389" s="6">
         <v>1</v>
       </c>
@@ -20563,7 +20562,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="390" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:16">
       <c r="A390" s="6">
         <v>1</v>
       </c>
@@ -20613,7 +20612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="391" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:16">
       <c r="A391" s="6">
         <v>1</v>
       </c>
@@ -20663,7 +20662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="392" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:16">
       <c r="A392" s="6">
         <v>1</v>
       </c>
@@ -20713,7 +20712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="393" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:16">
       <c r="A393" s="6">
         <v>1</v>
       </c>
@@ -20763,7 +20762,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="394" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:16">
       <c r="A394" s="6">
         <v>1</v>
       </c>
@@ -20813,7 +20812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="395" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:16">
       <c r="A395" s="6">
         <v>1</v>
       </c>
@@ -20863,7 +20862,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="396" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:16">
       <c r="A396" s="6">
         <v>1</v>
       </c>
@@ -20913,7 +20912,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="397" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:16">
       <c r="A397" s="6">
         <v>1</v>
       </c>
@@ -20963,7 +20962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="398" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:16">
       <c r="A398" s="6">
         <v>1</v>
       </c>
@@ -21013,7 +21012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="399" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:16">
       <c r="A399" s="6">
         <v>1</v>
       </c>
@@ -21063,7 +21062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="400" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:16">
       <c r="A400" s="6">
         <v>1</v>
       </c>
@@ -21113,7 +21112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="401" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:16">
       <c r="A401" s="6">
         <v>1</v>
       </c>
@@ -21163,7 +21162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="402" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:16">
       <c r="A402" s="7">
         <v>1</v>
       </c>
@@ -21223,34 +21222,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" customWidth="1"/>
+    <col min="14" max="14" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -21300,7 +21299,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>1</v>
       </c>
@@ -21350,7 +21349,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>1</v>
       </c>
@@ -21400,7 +21399,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>1</v>
       </c>
@@ -21450,7 +21449,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>1</v>
       </c>
@@ -21500,7 +21499,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>1</v>
       </c>
@@ -21550,7 +21549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>1</v>
       </c>
@@ -21600,7 +21599,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>1</v>
       </c>
@@ -21650,7 +21649,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>1</v>
       </c>
@@ -21700,7 +21699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>1</v>
       </c>
@@ -21750,7 +21749,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>1</v>
       </c>
@@ -21800,7 +21799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>1</v>
       </c>
@@ -21850,7 +21849,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>1</v>
       </c>
@@ -21900,7 +21899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>1</v>
       </c>
@@ -21950,7 +21949,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>1</v>
       </c>
@@ -22000,7 +21999,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16">
       <c r="A16">
         <v>1</v>
       </c>
@@ -22050,7 +22049,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16">
       <c r="A17">
         <v>1</v>
       </c>
@@ -22100,7 +22099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16">
       <c r="A18">
         <v>1</v>
       </c>
@@ -22150,7 +22149,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16">
       <c r="A19">
         <v>1</v>
       </c>
@@ -22200,7 +22199,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16">
       <c r="A20">
         <v>1</v>
       </c>
@@ -22250,7 +22249,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16">
       <c r="A21">
         <v>1</v>
       </c>
@@ -22300,7 +22299,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16">
       <c r="A22">
         <v>1</v>
       </c>
@@ -22350,7 +22349,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16">
       <c r="A23">
         <v>1</v>
       </c>
@@ -22400,7 +22399,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16">
       <c r="A24">
         <v>1</v>
       </c>
@@ -22450,7 +22449,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16">
       <c r="A25">
         <v>1</v>
       </c>
@@ -22500,7 +22499,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16">
       <c r="A26">
         <v>1</v>
       </c>
@@ -22550,7 +22549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16">
       <c r="A27">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
demolition logic added (to be discussed)
</commit_message>
<xml_diff>
--- a/projects/test_building/input/SimulatorScenarios.xlsx
+++ b/projects/test_building/input/SimulatorScenarios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yus\Documents\code\3E\RenderNew\projects\test_building\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4440022D-3757-BE46-BB9D-59947C5358B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="765" windowWidth="16380" windowHeight="8205" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="2" r:id="rId1"/>
@@ -85,8 +86,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -612,75 +613,75 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:P2" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
-  <autoFilter ref="A1:P2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:P2" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="A1:P2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="id" dataDxfId="33"/>
-    <tableColumn id="2" name="start_year" dataDxfId="32"/>
-    <tableColumn id="3" name="end_year" dataDxfId="31"/>
-    <tableColumn id="4" name="id_region" dataDxfId="30"/>
-    <tableColumn id="5" name="building_num_min" dataDxfId="29"/>
-    <tableColumn id="6" name="building_num_max" dataDxfId="28"/>
-    <tableColumn id="7" name="optimal_heating_behavior_prob" dataDxfId="27"/>
-    <tableColumn id="8" name="id_scenario_energy_price_wholesale" dataDxfId="26"/>
-    <tableColumn id="9" name="id_scenario_energy_price_tax_rate" dataDxfId="25"/>
-    <tableColumn id="10" name="id_scenario_energy_price_mark_up" dataDxfId="24"/>
-    <tableColumn id="11" name="id_scenario_energy_price_co2_emission" dataDxfId="23"/>
-    <tableColumn id="12" name="id_scenario_energy_emission_factor" dataDxfId="22"/>
-    <tableColumn id="15" name="renovation_mandatory" dataDxfId="21"/>
-    <tableColumn id="16" name="heating_technology_mandatory" dataDxfId="20"/>
-    <tableColumn id="13" name="name" dataDxfId="19"/>
-    <tableColumn id="14" name="comment" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="start_year" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="end_year" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_region" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="building_num_min" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="building_num_max" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="22"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="renovation_mandatory" dataDxfId="21"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="heating_technology_mandatory" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="name" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="comment" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:P402" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:P402"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:P402" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:P402" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="id" dataDxfId="15"/>
-    <tableColumn id="2" name="start_year" dataDxfId="14"/>
-    <tableColumn id="3" name="end_year" dataDxfId="13"/>
-    <tableColumn id="4" name="id_region" dataDxfId="12"/>
-    <tableColumn id="5" name="building_num_min" dataDxfId="11"/>
-    <tableColumn id="6" name="building_num_max" dataDxfId="10"/>
-    <tableColumn id="7" name="optimal_heating_behavior_prob" dataDxfId="9"/>
-    <tableColumn id="8" name="id_scenario_energy_price_wholesale" dataDxfId="8"/>
-    <tableColumn id="9" name="id_scenario_energy_price_tax_rate" dataDxfId="7"/>
-    <tableColumn id="10" name="id_scenario_energy_price_mark_up" dataDxfId="6"/>
-    <tableColumn id="11" name="id_scenario_energy_price_co2_emission" dataDxfId="5"/>
-    <tableColumn id="12" name="id_scenario_energy_emission_factor" dataDxfId="4"/>
-    <tableColumn id="15" name="renovation_mandatory" dataDxfId="3"/>
-    <tableColumn id="16" name="heating_technology_mandatory" dataDxfId="2"/>
-    <tableColumn id="13" name="name" dataDxfId="1"/>
-    <tableColumn id="14" name="comment" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="start_year" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="end_year" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="id_region" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="building_num_min" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="building_num_max" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="renovation_mandatory" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="heating_technology_mandatory" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="name" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:P27" totalsRowShown="0">
-  <autoFilter ref="A1:P27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:P27" totalsRowShown="0">
+  <autoFilter ref="A1:P27" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="id"/>
-    <tableColumn id="2" name="start_year"/>
-    <tableColumn id="3" name="end_year"/>
-    <tableColumn id="4" name="id_region"/>
-    <tableColumn id="5" name="building_num_min"/>
-    <tableColumn id="6" name="building_num_max"/>
-    <tableColumn id="7" name="optimal_heating_behavior_prob"/>
-    <tableColumn id="8" name="id_scenario_energy_price_wholesale"/>
-    <tableColumn id="9" name="id_scenario_energy_price_tax_rate"/>
-    <tableColumn id="10" name="id_scenario_energy_price_mark_up"/>
-    <tableColumn id="11" name="id_scenario_energy_price_co2_emission"/>
-    <tableColumn id="12" name="id_scenario_energy_emission_factor"/>
-    <tableColumn id="13" name="renovation_mandatory"/>
-    <tableColumn id="14" name="heating_technology_mandatory"/>
-    <tableColumn id="15" name="name"/>
-    <tableColumn id="16" name="comment"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="start_year"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="end_year"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="id_region"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="building_num_min"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="building_num_max"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="optimal_heating_behavior_prob"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="id_scenario_energy_price_wholesale"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="id_scenario_energy_price_tax_rate"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="id_scenario_energy_price_mark_up"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="id_scenario_energy_price_co2_emission"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="id_scenario_energy_emission_factor"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="renovation_mandatory"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0200-00000E000000}" name="heating_technology_mandatory"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0200-00000F000000}" name="name"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0200-000010000000}" name="comment"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -948,34 +949,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1025,7 +1026,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1039,10 +1040,10 @@
         <v>9010101</v>
       </c>
       <c r="E2" s="6">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F2" s="6">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="G2" s="6">
         <v>1</v>
@@ -1085,34 +1086,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P402"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1162,7 +1163,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1212,7 +1213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1262,7 +1263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -1312,7 +1313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -1362,7 +1363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -1412,7 +1413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>1</v>
       </c>
@@ -1462,7 +1463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -1512,7 +1513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>1</v>
       </c>
@@ -1562,7 +1563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>1</v>
       </c>
@@ -1612,7 +1613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>1</v>
       </c>
@@ -1662,7 +1663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>1</v>
       </c>
@@ -1712,7 +1713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>1</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>1</v>
       </c>
@@ -1812,7 +1813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>1</v>
       </c>
@@ -1862,7 +1863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>1</v>
       </c>
@@ -1912,7 +1913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>1</v>
       </c>
@@ -1962,7 +1963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>1</v>
       </c>
@@ -2012,7 +2013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>1</v>
       </c>
@@ -2062,7 +2063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>1</v>
       </c>
@@ -2112,7 +2113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>1</v>
       </c>
@@ -2162,7 +2163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>1</v>
       </c>
@@ -2212,7 +2213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>1</v>
       </c>
@@ -2262,7 +2263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>1</v>
       </c>
@@ -2312,7 +2313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>1</v>
       </c>
@@ -2362,7 +2363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>1</v>
       </c>
@@ -2412,7 +2413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>1</v>
       </c>
@@ -2462,7 +2463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>1</v>
       </c>
@@ -2512,7 +2513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>1</v>
       </c>
@@ -2562,7 +2563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>1</v>
       </c>
@@ -2612,7 +2613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>1</v>
       </c>
@@ -2662,7 +2663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>1</v>
       </c>
@@ -2712,7 +2713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>1</v>
       </c>
@@ -2762,7 +2763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>1</v>
       </c>
@@ -2812,7 +2813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>1</v>
       </c>
@@ -2862,7 +2863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>1</v>
       </c>
@@ -2912,7 +2913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>1</v>
       </c>
@@ -2962,7 +2963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>1</v>
       </c>
@@ -3012,7 +3013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>1</v>
       </c>
@@ -3062,7 +3063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>1</v>
       </c>
@@ -3112,7 +3113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>1</v>
       </c>
@@ -3162,7 +3163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>1</v>
       </c>
@@ -3212,7 +3213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>1</v>
       </c>
@@ -3262,7 +3263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>1</v>
       </c>
@@ -3312,7 +3313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>1</v>
       </c>
@@ -3362,7 +3363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>1</v>
       </c>
@@ -3412,7 +3413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>1</v>
       </c>
@@ -3462,7 +3463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>1</v>
       </c>
@@ -3512,7 +3513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>1</v>
       </c>
@@ -3562,7 +3563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>1</v>
       </c>
@@ -3612,7 +3613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>1</v>
       </c>
@@ -3662,7 +3663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>1</v>
       </c>
@@ -3712,7 +3713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>1</v>
       </c>
@@ -3762,7 +3763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>1</v>
       </c>
@@ -3812,7 +3813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
         <v>1</v>
       </c>
@@ -3862,7 +3863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>1</v>
       </c>
@@ -3912,7 +3913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
         <v>1</v>
       </c>
@@ -3962,7 +3963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
         <v>1</v>
       </c>
@@ -4012,7 +4013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>1</v>
       </c>
@@ -4062,7 +4063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>1</v>
       </c>
@@ -4112,7 +4113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>1</v>
       </c>
@@ -4162,7 +4163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
         <v>1</v>
       </c>
@@ -4212,7 +4213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>1</v>
       </c>
@@ -4262,7 +4263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>1</v>
       </c>
@@ -4312,7 +4313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>1</v>
       </c>
@@ -4362,7 +4363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
         <v>1</v>
       </c>
@@ -4412,7 +4413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="6">
         <v>1</v>
       </c>
@@ -4462,7 +4463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
         <v>1</v>
       </c>
@@ -4512,7 +4513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="6">
         <v>1</v>
       </c>
@@ -4562,7 +4563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>1</v>
       </c>
@@ -4612,7 +4613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="6">
         <v>1</v>
       </c>
@@ -4662,7 +4663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>1</v>
       </c>
@@ -4712,7 +4713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="6">
         <v>1</v>
       </c>
@@ -4762,7 +4763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
         <v>1</v>
       </c>
@@ -4812,7 +4813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" s="6">
         <v>1</v>
       </c>
@@ -4862,7 +4863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
         <v>1</v>
       </c>
@@ -4912,7 +4913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" s="6">
         <v>1</v>
       </c>
@@ -4962,7 +4963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="6">
         <v>1</v>
       </c>
@@ -5012,7 +5013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" s="6">
         <v>1</v>
       </c>
@@ -5062,7 +5063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" s="6">
         <v>1</v>
       </c>
@@ -5112,7 +5113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" s="6">
         <v>1</v>
       </c>
@@ -5162,7 +5163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="6">
         <v>1</v>
       </c>
@@ -5212,7 +5213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" s="6">
         <v>1</v>
       </c>
@@ -5262,7 +5263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" s="6">
         <v>1</v>
       </c>
@@ -5312,7 +5313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="6">
         <v>1</v>
       </c>
@@ -5362,7 +5363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="6">
         <v>1</v>
       </c>
@@ -5412,7 +5413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="6">
         <v>1</v>
       </c>
@@ -5462,7 +5463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="6">
         <v>1</v>
       </c>
@@ -5512,7 +5513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="6">
         <v>1</v>
       </c>
@@ -5562,7 +5563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="6">
         <v>1</v>
       </c>
@@ -5612,7 +5613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91" s="6">
         <v>1</v>
       </c>
@@ -5662,7 +5663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92" s="6">
         <v>1</v>
       </c>
@@ -5712,7 +5713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93" s="6">
         <v>1</v>
       </c>
@@ -5762,7 +5763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94" s="6">
         <v>1</v>
       </c>
@@ -5812,7 +5813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95" s="6">
         <v>1</v>
       </c>
@@ -5862,7 +5863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96" s="6">
         <v>1</v>
       </c>
@@ -5912,7 +5913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97" s="6">
         <v>1</v>
       </c>
@@ -5962,7 +5963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
         <v>1</v>
       </c>
@@ -6012,7 +6013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99" s="6">
         <v>1</v>
       </c>
@@ -6062,7 +6063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100" s="6">
         <v>1</v>
       </c>
@@ -6112,7 +6113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101" s="6">
         <v>1</v>
       </c>
@@ -6162,7 +6163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102" s="6">
         <v>1</v>
       </c>
@@ -6212,7 +6213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103" s="6">
         <v>1</v>
       </c>
@@ -6262,7 +6263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104" s="6">
         <v>1</v>
       </c>
@@ -6312,7 +6313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105" s="6">
         <v>1</v>
       </c>
@@ -6362,7 +6363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106" s="6">
         <v>1</v>
       </c>
@@ -6412,7 +6413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107" s="6">
         <v>1</v>
       </c>
@@ -6462,7 +6463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108" s="6">
         <v>1</v>
       </c>
@@ -6512,7 +6513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109" s="6">
         <v>1</v>
       </c>
@@ -6562,7 +6563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:16">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110" s="6">
         <v>1</v>
       </c>
@@ -6612,7 +6613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:16">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111" s="6">
         <v>1</v>
       </c>
@@ -6662,7 +6663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112" s="6">
         <v>1</v>
       </c>
@@ -6712,7 +6713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113" s="6">
         <v>1</v>
       </c>
@@ -6762,7 +6763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114" s="6">
         <v>1</v>
       </c>
@@ -6812,7 +6813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115" s="6">
         <v>1</v>
       </c>
@@ -6862,7 +6863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116" s="6">
         <v>1</v>
       </c>
@@ -6912,7 +6913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117" s="6">
         <v>1</v>
       </c>
@@ -6962,7 +6963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118" s="6">
         <v>1</v>
       </c>
@@ -7012,7 +7013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119" s="6">
         <v>1</v>
       </c>
@@ -7062,7 +7063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120" s="6">
         <v>1</v>
       </c>
@@ -7112,7 +7113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:16">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121" s="6">
         <v>1</v>
       </c>
@@ -7162,7 +7163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:16">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122" s="6">
         <v>1</v>
       </c>
@@ -7212,7 +7213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:16">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123" s="6">
         <v>1</v>
       </c>
@@ -7262,7 +7263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124" s="6">
         <v>1</v>
       </c>
@@ -7312,7 +7313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:16">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125" s="6">
         <v>1</v>
       </c>
@@ -7362,7 +7363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:16">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" s="6">
         <v>1</v>
       </c>
@@ -7412,7 +7413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:16">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" s="6">
         <v>1</v>
       </c>
@@ -7462,7 +7463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:16">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="6">
         <v>1</v>
       </c>
@@ -7512,7 +7513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:16">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="6">
         <v>1</v>
       </c>
@@ -7562,7 +7563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:16">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="6">
         <v>1</v>
       </c>
@@ -7612,7 +7613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:16">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="6">
         <v>1</v>
       </c>
@@ -7662,7 +7663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:16">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="6">
         <v>1</v>
       </c>
@@ -7712,7 +7713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:16">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="6">
         <v>1</v>
       </c>
@@ -7762,7 +7763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:16">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" s="6">
         <v>1</v>
       </c>
@@ -7812,7 +7813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:16">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="6">
         <v>1</v>
       </c>
@@ -7862,7 +7863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:16">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" s="6">
         <v>1</v>
       </c>
@@ -7912,7 +7913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:16">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" s="6">
         <v>1</v>
       </c>
@@ -7962,7 +7963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:16">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" s="6">
         <v>1</v>
       </c>
@@ -8012,7 +8013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:16">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" s="6">
         <v>1</v>
       </c>
@@ -8062,7 +8063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:16">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140" s="6">
         <v>1</v>
       </c>
@@ -8112,7 +8113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:16">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" s="6">
         <v>1</v>
       </c>
@@ -8162,7 +8163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:16">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" s="6">
         <v>1</v>
       </c>
@@ -8212,7 +8213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:16">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" s="6">
         <v>1</v>
       </c>
@@ -8262,7 +8263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:16">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" s="6">
         <v>1</v>
       </c>
@@ -8312,7 +8313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:16">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" s="6">
         <v>1</v>
       </c>
@@ -8362,7 +8363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:16">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" s="6">
         <v>1</v>
       </c>
@@ -8412,7 +8413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:16">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147" s="6">
         <v>1</v>
       </c>
@@ -8462,7 +8463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:16">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148" s="6">
         <v>1</v>
       </c>
@@ -8512,7 +8513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:16">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149" s="6">
         <v>1</v>
       </c>
@@ -8562,7 +8563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:16">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A150" s="6">
         <v>1</v>
       </c>
@@ -8612,7 +8613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:16">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151" s="6">
         <v>1</v>
       </c>
@@ -8662,7 +8663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:16">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152" s="6">
         <v>1</v>
       </c>
@@ -8712,7 +8713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:16">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153" s="6">
         <v>1</v>
       </c>
@@ -8762,7 +8763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:16">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154" s="6">
         <v>1</v>
       </c>
@@ -8812,7 +8813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:16">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155" s="6">
         <v>1</v>
       </c>
@@ -8862,7 +8863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:16">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156" s="6">
         <v>1</v>
       </c>
@@ -8912,7 +8913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:16">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A157" s="6">
         <v>1</v>
       </c>
@@ -8962,7 +8963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:16">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A158" s="6">
         <v>1</v>
       </c>
@@ -9012,7 +9013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:16">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A159" s="6">
         <v>1</v>
       </c>
@@ -9062,7 +9063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:16">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A160" s="6">
         <v>1</v>
       </c>
@@ -9112,7 +9113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:16">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A161" s="6">
         <v>1</v>
       </c>
@@ -9162,7 +9163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="162" spans="1:16">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A162" s="6">
         <v>1</v>
       </c>
@@ -9212,7 +9213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:16">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A163" s="6">
         <v>1</v>
       </c>
@@ -9262,7 +9263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:16">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A164" s="6">
         <v>1</v>
       </c>
@@ -9312,7 +9313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:16">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A165" s="6">
         <v>1</v>
       </c>
@@ -9362,7 +9363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:16">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A166" s="6">
         <v>1</v>
       </c>
@@ -9412,7 +9413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="1:16">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A167" s="6">
         <v>1</v>
       </c>
@@ -9462,7 +9463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:16">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A168" s="6">
         <v>1</v>
       </c>
@@ -9512,7 +9513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:16">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A169" s="6">
         <v>1</v>
       </c>
@@ -9562,7 +9563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:16">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A170" s="6">
         <v>1</v>
       </c>
@@ -9612,7 +9613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:16">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A171" s="6">
         <v>1</v>
       </c>
@@ -9662,7 +9663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="1:16">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A172" s="6">
         <v>1</v>
       </c>
@@ -9712,7 +9713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:16">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A173" s="6">
         <v>1</v>
       </c>
@@ -9762,7 +9763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:16">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A174" s="6">
         <v>1</v>
       </c>
@@ -9812,7 +9813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:16">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A175" s="6">
         <v>1</v>
       </c>
@@ -9862,7 +9863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="176" spans="1:16">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A176" s="6">
         <v>1</v>
       </c>
@@ -9912,7 +9913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:16">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A177" s="6">
         <v>1</v>
       </c>
@@ -9962,7 +9963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:16">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A178" s="6">
         <v>1</v>
       </c>
@@ -10012,7 +10013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:16">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A179" s="6">
         <v>1</v>
       </c>
@@ -10062,7 +10063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:16">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A180" s="6">
         <v>1</v>
       </c>
@@ -10112,7 +10113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:16">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A181" s="6">
         <v>1</v>
       </c>
@@ -10162,7 +10163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="182" spans="1:16">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A182" s="6">
         <v>1</v>
       </c>
@@ -10212,7 +10213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:16">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A183" s="6">
         <v>1</v>
       </c>
@@ -10262,7 +10263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:16">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A184" s="6">
         <v>1</v>
       </c>
@@ -10312,7 +10313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:16">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A185" s="6">
         <v>1</v>
       </c>
@@ -10362,7 +10363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="186" spans="1:16">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A186" s="6">
         <v>1</v>
       </c>
@@ -10412,7 +10413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:16">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A187" s="6">
         <v>1</v>
       </c>
@@ -10462,7 +10463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="188" spans="1:16">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A188" s="6">
         <v>1</v>
       </c>
@@ -10512,7 +10513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="189" spans="1:16">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A189" s="6">
         <v>1</v>
       </c>
@@ -10562,7 +10563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="190" spans="1:16">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A190" s="6">
         <v>1</v>
       </c>
@@ -10612,7 +10613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="191" spans="1:16">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A191" s="6">
         <v>1</v>
       </c>
@@ -10662,7 +10663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="192" spans="1:16">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A192" s="6">
         <v>1</v>
       </c>
@@ -10712,7 +10713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="1:16">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A193" s="6">
         <v>1</v>
       </c>
@@ -10762,7 +10763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="194" spans="1:16">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A194" s="6">
         <v>1</v>
       </c>
@@ -10812,7 +10813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="195" spans="1:16">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A195" s="6">
         <v>1</v>
       </c>
@@ -10862,7 +10863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:16">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A196" s="6">
         <v>1</v>
       </c>
@@ -10912,7 +10913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="197" spans="1:16">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A197" s="6">
         <v>1</v>
       </c>
@@ -10962,7 +10963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="198" spans="1:16">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A198" s="6">
         <v>1</v>
       </c>
@@ -11012,7 +11013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="199" spans="1:16">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A199" s="6">
         <v>1</v>
       </c>
@@ -11062,7 +11063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="200" spans="1:16">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A200" s="6">
         <v>1</v>
       </c>
@@ -11112,7 +11113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="201" spans="1:16">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A201" s="6">
         <v>1</v>
       </c>
@@ -11162,7 +11163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="202" spans="1:16">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A202" s="6">
         <v>1</v>
       </c>
@@ -11212,7 +11213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="203" spans="1:16">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A203" s="6">
         <v>1</v>
       </c>
@@ -11262,7 +11263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="204" spans="1:16">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A204" s="6">
         <v>1</v>
       </c>
@@ -11312,7 +11313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="205" spans="1:16">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A205" s="6">
         <v>1</v>
       </c>
@@ -11362,7 +11363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="206" spans="1:16">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A206" s="6">
         <v>1</v>
       </c>
@@ -11412,7 +11413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="207" spans="1:16">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A207" s="6">
         <v>1</v>
       </c>
@@ -11462,7 +11463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:16">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A208" s="6">
         <v>1</v>
       </c>
@@ -11512,7 +11513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="209" spans="1:16">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A209" s="6">
         <v>1</v>
       </c>
@@ -11562,7 +11563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="210" spans="1:16">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A210" s="6">
         <v>1</v>
       </c>
@@ -11612,7 +11613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="211" spans="1:16">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A211" s="6">
         <v>1</v>
       </c>
@@ -11662,7 +11663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="212" spans="1:16">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A212" s="6">
         <v>1</v>
       </c>
@@ -11712,7 +11713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="213" spans="1:16">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A213" s="6">
         <v>1</v>
       </c>
@@ -11762,7 +11763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="214" spans="1:16">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A214" s="6">
         <v>1</v>
       </c>
@@ -11812,7 +11813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="215" spans="1:16">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A215" s="6">
         <v>1</v>
       </c>
@@ -11862,7 +11863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="216" spans="1:16">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A216" s="6">
         <v>1</v>
       </c>
@@ -11912,7 +11913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="217" spans="1:16">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A217" s="6">
         <v>1</v>
       </c>
@@ -11962,7 +11963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="218" spans="1:16">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A218" s="6">
         <v>1</v>
       </c>
@@ -12012,7 +12013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="219" spans="1:16">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A219" s="6">
         <v>1</v>
       </c>
@@ -12062,7 +12063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="220" spans="1:16">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A220" s="6">
         <v>1</v>
       </c>
@@ -12112,7 +12113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="221" spans="1:16">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A221" s="6">
         <v>1</v>
       </c>
@@ -12162,7 +12163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="222" spans="1:16">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A222" s="6">
         <v>1</v>
       </c>
@@ -12212,7 +12213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="223" spans="1:16">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A223" s="6">
         <v>1</v>
       </c>
@@ -12262,7 +12263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="224" spans="1:16">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A224" s="6">
         <v>1</v>
       </c>
@@ -12312,7 +12313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="225" spans="1:16">
+    <row r="225" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A225" s="6">
         <v>1</v>
       </c>
@@ -12362,7 +12363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="226" spans="1:16">
+    <row r="226" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A226" s="6">
         <v>1</v>
       </c>
@@ -12412,7 +12413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="227" spans="1:16">
+    <row r="227" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A227" s="6">
         <v>1</v>
       </c>
@@ -12462,7 +12463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="228" spans="1:16">
+    <row r="228" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A228" s="6">
         <v>1</v>
       </c>
@@ -12512,7 +12513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="229" spans="1:16">
+    <row r="229" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A229" s="6">
         <v>1</v>
       </c>
@@ -12562,7 +12563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="230" spans="1:16">
+    <row r="230" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A230" s="6">
         <v>1</v>
       </c>
@@ -12612,7 +12613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="231" spans="1:16">
+    <row r="231" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A231" s="6">
         <v>1</v>
       </c>
@@ -12662,7 +12663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="232" spans="1:16">
+    <row r="232" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A232" s="6">
         <v>1</v>
       </c>
@@ -12712,7 +12713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="1:16">
+    <row r="233" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A233" s="6">
         <v>1</v>
       </c>
@@ -12762,7 +12763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="234" spans="1:16">
+    <row r="234" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A234" s="6">
         <v>1</v>
       </c>
@@ -12812,7 +12813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="235" spans="1:16">
+    <row r="235" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A235" s="6">
         <v>1</v>
       </c>
@@ -12862,7 +12863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="236" spans="1:16">
+    <row r="236" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A236" s="6">
         <v>1</v>
       </c>
@@ -12912,7 +12913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="237" spans="1:16">
+    <row r="237" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A237" s="6">
         <v>1</v>
       </c>
@@ -12962,7 +12963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="238" spans="1:16">
+    <row r="238" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A238" s="6">
         <v>1</v>
       </c>
@@ -13012,7 +13013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="239" spans="1:16">
+    <row r="239" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A239" s="6">
         <v>1</v>
       </c>
@@ -13062,7 +13063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="240" spans="1:16">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A240" s="6">
         <v>1</v>
       </c>
@@ -13112,7 +13113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="241" spans="1:16">
+    <row r="241" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A241" s="6">
         <v>1</v>
       </c>
@@ -13162,7 +13163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="242" spans="1:16">
+    <row r="242" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A242" s="6">
         <v>1</v>
       </c>
@@ -13212,7 +13213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="243" spans="1:16">
+    <row r="243" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A243" s="6">
         <v>1</v>
       </c>
@@ -13262,7 +13263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="244" spans="1:16">
+    <row r="244" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A244" s="6">
         <v>1</v>
       </c>
@@ -13312,7 +13313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="245" spans="1:16">
+    <row r="245" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A245" s="6">
         <v>1</v>
       </c>
@@ -13362,7 +13363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="246" spans="1:16">
+    <row r="246" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A246" s="6">
         <v>1</v>
       </c>
@@ -13412,7 +13413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="247" spans="1:16">
+    <row r="247" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A247" s="6">
         <v>1</v>
       </c>
@@ -13462,7 +13463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="248" spans="1:16">
+    <row r="248" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A248" s="6">
         <v>1</v>
       </c>
@@ -13512,7 +13513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="249" spans="1:16">
+    <row r="249" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A249" s="6">
         <v>1</v>
       </c>
@@ -13562,7 +13563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="250" spans="1:16">
+    <row r="250" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A250" s="6">
         <v>1</v>
       </c>
@@ -13612,7 +13613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="251" spans="1:16">
+    <row r="251" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A251" s="6">
         <v>1</v>
       </c>
@@ -13662,7 +13663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="252" spans="1:16">
+    <row r="252" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A252" s="6">
         <v>1</v>
       </c>
@@ -13712,7 +13713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="253" spans="1:16">
+    <row r="253" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A253" s="6">
         <v>1</v>
       </c>
@@ -13762,7 +13763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="254" spans="1:16">
+    <row r="254" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A254" s="6">
         <v>1</v>
       </c>
@@ -13812,7 +13813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="255" spans="1:16">
+    <row r="255" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A255" s="6">
         <v>1</v>
       </c>
@@ -13862,7 +13863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="256" spans="1:16">
+    <row r="256" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A256" s="6">
         <v>1</v>
       </c>
@@ -13912,7 +13913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="257" spans="1:16">
+    <row r="257" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A257" s="6">
         <v>1</v>
       </c>
@@ -13962,7 +13963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="258" spans="1:16">
+    <row r="258" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A258" s="6">
         <v>1</v>
       </c>
@@ -14012,7 +14013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="259" spans="1:16">
+    <row r="259" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A259" s="6">
         <v>1</v>
       </c>
@@ -14062,7 +14063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="260" spans="1:16">
+    <row r="260" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A260" s="6">
         <v>1</v>
       </c>
@@ -14112,7 +14113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="261" spans="1:16">
+    <row r="261" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A261" s="6">
         <v>1</v>
       </c>
@@ -14162,7 +14163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="262" spans="1:16">
+    <row r="262" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A262" s="6">
         <v>1</v>
       </c>
@@ -14212,7 +14213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="263" spans="1:16">
+    <row r="263" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A263" s="6">
         <v>1</v>
       </c>
@@ -14262,7 +14263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="264" spans="1:16">
+    <row r="264" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A264" s="6">
         <v>1</v>
       </c>
@@ -14312,7 +14313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="265" spans="1:16">
+    <row r="265" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A265" s="6">
         <v>1</v>
       </c>
@@ -14362,7 +14363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="266" spans="1:16">
+    <row r="266" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A266" s="6">
         <v>1</v>
       </c>
@@ -14412,7 +14413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="267" spans="1:16">
+    <row r="267" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A267" s="6">
         <v>1</v>
       </c>
@@ -14462,7 +14463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="268" spans="1:16">
+    <row r="268" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A268" s="6">
         <v>1</v>
       </c>
@@ -14512,7 +14513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="269" spans="1:16">
+    <row r="269" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A269" s="6">
         <v>1</v>
       </c>
@@ -14562,7 +14563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="270" spans="1:16">
+    <row r="270" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A270" s="6">
         <v>1</v>
       </c>
@@ -14612,7 +14613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="271" spans="1:16">
+    <row r="271" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A271" s="6">
         <v>1</v>
       </c>
@@ -14662,7 +14663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="272" spans="1:16">
+    <row r="272" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A272" s="6">
         <v>1</v>
       </c>
@@ -14712,7 +14713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="273" spans="1:16">
+    <row r="273" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A273" s="6">
         <v>1</v>
       </c>
@@ -14762,7 +14763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="274" spans="1:16">
+    <row r="274" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A274" s="6">
         <v>1</v>
       </c>
@@ -14812,7 +14813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="275" spans="1:16">
+    <row r="275" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A275" s="6">
         <v>1</v>
       </c>
@@ -14862,7 +14863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="276" spans="1:16">
+    <row r="276" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A276" s="6">
         <v>1</v>
       </c>
@@ -14912,7 +14913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="277" spans="1:16">
+    <row r="277" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A277" s="6">
         <v>1</v>
       </c>
@@ -14962,7 +14963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="278" spans="1:16">
+    <row r="278" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A278" s="6">
         <v>1</v>
       </c>
@@ -15012,7 +15013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="279" spans="1:16">
+    <row r="279" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A279" s="6">
         <v>1</v>
       </c>
@@ -15062,7 +15063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="280" spans="1:16">
+    <row r="280" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A280" s="6">
         <v>1</v>
       </c>
@@ -15112,7 +15113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="281" spans="1:16">
+    <row r="281" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A281" s="6">
         <v>1</v>
       </c>
@@ -15162,7 +15163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="282" spans="1:16">
+    <row r="282" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A282" s="6">
         <v>1</v>
       </c>
@@ -15212,7 +15213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="283" spans="1:16">
+    <row r="283" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A283" s="6">
         <v>1</v>
       </c>
@@ -15262,7 +15263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="284" spans="1:16">
+    <row r="284" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A284" s="6">
         <v>1</v>
       </c>
@@ -15312,7 +15313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="285" spans="1:16">
+    <row r="285" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A285" s="6">
         <v>1</v>
       </c>
@@ -15362,7 +15363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="286" spans="1:16">
+    <row r="286" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A286" s="6">
         <v>1</v>
       </c>
@@ -15412,7 +15413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="287" spans="1:16">
+    <row r="287" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A287" s="6">
         <v>1</v>
       </c>
@@ -15462,7 +15463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="288" spans="1:16">
+    <row r="288" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A288" s="6">
         <v>1</v>
       </c>
@@ -15512,7 +15513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="289" spans="1:16">
+    <row r="289" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A289" s="6">
         <v>1</v>
       </c>
@@ -15562,7 +15563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="290" spans="1:16">
+    <row r="290" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A290" s="6">
         <v>1</v>
       </c>
@@ -15612,7 +15613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="291" spans="1:16">
+    <row r="291" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A291" s="6">
         <v>1</v>
       </c>
@@ -15662,7 +15663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="292" spans="1:16">
+    <row r="292" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A292" s="6">
         <v>1</v>
       </c>
@@ -15712,7 +15713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="293" spans="1:16">
+    <row r="293" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A293" s="6">
         <v>1</v>
       </c>
@@ -15762,7 +15763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="294" spans="1:16">
+    <row r="294" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A294" s="6">
         <v>1</v>
       </c>
@@ -15812,7 +15813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="295" spans="1:16">
+    <row r="295" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A295" s="6">
         <v>1</v>
       </c>
@@ -15862,7 +15863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="296" spans="1:16">
+    <row r="296" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A296" s="6">
         <v>1</v>
       </c>
@@ -15912,7 +15913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="297" spans="1:16">
+    <row r="297" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A297" s="6">
         <v>1</v>
       </c>
@@ -15962,7 +15963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="298" spans="1:16">
+    <row r="298" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A298" s="6">
         <v>1</v>
       </c>
@@ -16012,7 +16013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="299" spans="1:16">
+    <row r="299" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A299" s="6">
         <v>1</v>
       </c>
@@ -16062,7 +16063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="300" spans="1:16">
+    <row r="300" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A300" s="6">
         <v>1</v>
       </c>
@@ -16112,7 +16113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="301" spans="1:16">
+    <row r="301" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A301" s="6">
         <v>1</v>
       </c>
@@ -16162,7 +16163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="302" spans="1:16">
+    <row r="302" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A302" s="6">
         <v>1</v>
       </c>
@@ -16212,7 +16213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="303" spans="1:16">
+    <row r="303" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A303" s="6">
         <v>1</v>
       </c>
@@ -16262,7 +16263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="304" spans="1:16">
+    <row r="304" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A304" s="6">
         <v>1</v>
       </c>
@@ -16312,7 +16313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="305" spans="1:16">
+    <row r="305" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A305" s="6">
         <v>1</v>
       </c>
@@ -16362,7 +16363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="306" spans="1:16">
+    <row r="306" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A306" s="6">
         <v>1</v>
       </c>
@@ -16412,7 +16413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="307" spans="1:16">
+    <row r="307" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A307" s="6">
         <v>1</v>
       </c>
@@ -16462,7 +16463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="308" spans="1:16">
+    <row r="308" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A308" s="6">
         <v>1</v>
       </c>
@@ -16512,7 +16513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="309" spans="1:16">
+    <row r="309" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A309" s="6">
         <v>1</v>
       </c>
@@ -16562,7 +16563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="310" spans="1:16">
+    <row r="310" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A310" s="6">
         <v>1</v>
       </c>
@@ -16612,7 +16613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="311" spans="1:16">
+    <row r="311" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A311" s="6">
         <v>1</v>
       </c>
@@ -16662,7 +16663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="312" spans="1:16">
+    <row r="312" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A312" s="6">
         <v>1</v>
       </c>
@@ -16712,7 +16713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="313" spans="1:16">
+    <row r="313" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A313" s="6">
         <v>1</v>
       </c>
@@ -16762,7 +16763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="314" spans="1:16">
+    <row r="314" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A314" s="6">
         <v>1</v>
       </c>
@@ -16812,7 +16813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="315" spans="1:16">
+    <row r="315" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A315" s="6">
         <v>1</v>
       </c>
@@ -16862,7 +16863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="316" spans="1:16">
+    <row r="316" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A316" s="6">
         <v>1</v>
       </c>
@@ -16912,7 +16913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="317" spans="1:16">
+    <row r="317" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A317" s="6">
         <v>1</v>
       </c>
@@ -16962,7 +16963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="318" spans="1:16">
+    <row r="318" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A318" s="6">
         <v>1</v>
       </c>
@@ -17012,7 +17013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="319" spans="1:16">
+    <row r="319" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A319" s="6">
         <v>1</v>
       </c>
@@ -17062,7 +17063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="320" spans="1:16">
+    <row r="320" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A320" s="6">
         <v>1</v>
       </c>
@@ -17112,7 +17113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="321" spans="1:16">
+    <row r="321" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A321" s="6">
         <v>1</v>
       </c>
@@ -17162,7 +17163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="322" spans="1:16">
+    <row r="322" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A322" s="6">
         <v>1</v>
       </c>
@@ -17212,7 +17213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="323" spans="1:16">
+    <row r="323" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A323" s="6">
         <v>1</v>
       </c>
@@ -17262,7 +17263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="324" spans="1:16">
+    <row r="324" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A324" s="6">
         <v>1</v>
       </c>
@@ -17312,7 +17313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="325" spans="1:16">
+    <row r="325" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A325" s="6">
         <v>1</v>
       </c>
@@ -17362,7 +17363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="326" spans="1:16">
+    <row r="326" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A326" s="6">
         <v>1</v>
       </c>
@@ -17412,7 +17413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="327" spans="1:16">
+    <row r="327" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A327" s="6">
         <v>1</v>
       </c>
@@ -17462,7 +17463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="328" spans="1:16">
+    <row r="328" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A328" s="6">
         <v>1</v>
       </c>
@@ -17512,7 +17513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="329" spans="1:16">
+    <row r="329" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A329" s="6">
         <v>1</v>
       </c>
@@ -17562,7 +17563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="330" spans="1:16">
+    <row r="330" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A330" s="6">
         <v>1</v>
       </c>
@@ -17612,7 +17613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="331" spans="1:16">
+    <row r="331" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A331" s="6">
         <v>1</v>
       </c>
@@ -17662,7 +17663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="332" spans="1:16">
+    <row r="332" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A332" s="6">
         <v>1</v>
       </c>
@@ -17712,7 +17713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="333" spans="1:16">
+    <row r="333" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A333" s="6">
         <v>1</v>
       </c>
@@ -17762,7 +17763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="334" spans="1:16">
+    <row r="334" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A334" s="6">
         <v>1</v>
       </c>
@@ -17812,7 +17813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="335" spans="1:16">
+    <row r="335" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A335" s="6">
         <v>1</v>
       </c>
@@ -17862,7 +17863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="336" spans="1:16">
+    <row r="336" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A336" s="6">
         <v>1</v>
       </c>
@@ -17912,7 +17913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="337" spans="1:16">
+    <row r="337" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A337" s="6">
         <v>1</v>
       </c>
@@ -17962,7 +17963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="338" spans="1:16">
+    <row r="338" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A338" s="6">
         <v>1</v>
       </c>
@@ -18012,7 +18013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="339" spans="1:16">
+    <row r="339" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A339" s="6">
         <v>1</v>
       </c>
@@ -18062,7 +18063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="340" spans="1:16">
+    <row r="340" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A340" s="6">
         <v>1</v>
       </c>
@@ -18112,7 +18113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="341" spans="1:16">
+    <row r="341" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A341" s="6">
         <v>1</v>
       </c>
@@ -18162,7 +18163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="342" spans="1:16">
+    <row r="342" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A342" s="6">
         <v>1</v>
       </c>
@@ -18212,7 +18213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="343" spans="1:16">
+    <row r="343" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A343" s="6">
         <v>1</v>
       </c>
@@ -18262,7 +18263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="344" spans="1:16">
+    <row r="344" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A344" s="6">
         <v>1</v>
       </c>
@@ -18312,7 +18313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="345" spans="1:16">
+    <row r="345" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A345" s="6">
         <v>1</v>
       </c>
@@ -18362,7 +18363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="346" spans="1:16">
+    <row r="346" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A346" s="6">
         <v>1</v>
       </c>
@@ -18412,7 +18413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="347" spans="1:16">
+    <row r="347" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A347" s="6">
         <v>1</v>
       </c>
@@ -18462,7 +18463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="348" spans="1:16">
+    <row r="348" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A348" s="6">
         <v>1</v>
       </c>
@@ -18512,7 +18513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="349" spans="1:16">
+    <row r="349" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A349" s="6">
         <v>1</v>
       </c>
@@ -18562,7 +18563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="350" spans="1:16">
+    <row r="350" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A350" s="6">
         <v>1</v>
       </c>
@@ -18612,7 +18613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="351" spans="1:16">
+    <row r="351" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A351" s="6">
         <v>1</v>
       </c>
@@ -18662,7 +18663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="352" spans="1:16">
+    <row r="352" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A352" s="6">
         <v>1</v>
       </c>
@@ -18712,7 +18713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="353" spans="1:16">
+    <row r="353" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A353" s="6">
         <v>1</v>
       </c>
@@ -18762,7 +18763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="354" spans="1:16">
+    <row r="354" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A354" s="6">
         <v>1</v>
       </c>
@@ -18812,7 +18813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="355" spans="1:16">
+    <row r="355" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A355" s="6">
         <v>1</v>
       </c>
@@ -18862,7 +18863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="356" spans="1:16">
+    <row r="356" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A356" s="6">
         <v>1</v>
       </c>
@@ -18912,7 +18913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="357" spans="1:16">
+    <row r="357" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A357" s="6">
         <v>1</v>
       </c>
@@ -18962,7 +18963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="358" spans="1:16">
+    <row r="358" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A358" s="6">
         <v>1</v>
       </c>
@@ -19012,7 +19013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="359" spans="1:16">
+    <row r="359" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A359" s="6">
         <v>1</v>
       </c>
@@ -19062,7 +19063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="360" spans="1:16">
+    <row r="360" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A360" s="6">
         <v>1</v>
       </c>
@@ -19112,7 +19113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="361" spans="1:16">
+    <row r="361" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A361" s="6">
         <v>1</v>
       </c>
@@ -19162,7 +19163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="362" spans="1:16">
+    <row r="362" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A362" s="6">
         <v>1</v>
       </c>
@@ -19212,7 +19213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="363" spans="1:16">
+    <row r="363" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A363" s="6">
         <v>1</v>
       </c>
@@ -19262,7 +19263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="364" spans="1:16">
+    <row r="364" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A364" s="6">
         <v>1</v>
       </c>
@@ -19312,7 +19313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="365" spans="1:16">
+    <row r="365" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A365" s="6">
         <v>1</v>
       </c>
@@ -19362,7 +19363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="366" spans="1:16">
+    <row r="366" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A366" s="6">
         <v>1</v>
       </c>
@@ -19412,7 +19413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="367" spans="1:16">
+    <row r="367" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A367" s="6">
         <v>1</v>
       </c>
@@ -19462,7 +19463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="368" spans="1:16">
+    <row r="368" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A368" s="6">
         <v>1</v>
       </c>
@@ -19512,7 +19513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="369" spans="1:16">
+    <row r="369" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A369" s="6">
         <v>1</v>
       </c>
@@ -19562,7 +19563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="370" spans="1:16">
+    <row r="370" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A370" s="6">
         <v>1</v>
       </c>
@@ -19612,7 +19613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="371" spans="1:16">
+    <row r="371" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A371" s="6">
         <v>1</v>
       </c>
@@ -19662,7 +19663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="372" spans="1:16">
+    <row r="372" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A372" s="6">
         <v>1</v>
       </c>
@@ -19712,7 +19713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="373" spans="1:16">
+    <row r="373" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A373" s="6">
         <v>1</v>
       </c>
@@ -19762,7 +19763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="374" spans="1:16">
+    <row r="374" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A374" s="6">
         <v>1</v>
       </c>
@@ -19812,7 +19813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="375" spans="1:16">
+    <row r="375" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A375" s="6">
         <v>1</v>
       </c>
@@ -19862,7 +19863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="376" spans="1:16">
+    <row r="376" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A376" s="6">
         <v>1</v>
       </c>
@@ -19912,7 +19913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="377" spans="1:16">
+    <row r="377" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A377" s="6">
         <v>1</v>
       </c>
@@ -19962,7 +19963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="378" spans="1:16">
+    <row r="378" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A378" s="6">
         <v>1</v>
       </c>
@@ -20012,7 +20013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="379" spans="1:16">
+    <row r="379" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A379" s="6">
         <v>1</v>
       </c>
@@ -20062,7 +20063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="380" spans="1:16">
+    <row r="380" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A380" s="6">
         <v>1</v>
       </c>
@@ -20112,7 +20113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="381" spans="1:16">
+    <row r="381" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A381" s="6">
         <v>1</v>
       </c>
@@ -20162,7 +20163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="382" spans="1:16">
+    <row r="382" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A382" s="6">
         <v>1</v>
       </c>
@@ -20212,7 +20213,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="383" spans="1:16">
+    <row r="383" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A383" s="6">
         <v>1</v>
       </c>
@@ -20262,7 +20263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="384" spans="1:16">
+    <row r="384" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A384" s="6">
         <v>1</v>
       </c>
@@ -20312,7 +20313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="385" spans="1:16">
+    <row r="385" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A385" s="6">
         <v>1</v>
       </c>
@@ -20362,7 +20363,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="386" spans="1:16">
+    <row r="386" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A386" s="6">
         <v>1</v>
       </c>
@@ -20412,7 +20413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="387" spans="1:16">
+    <row r="387" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A387" s="6">
         <v>1</v>
       </c>
@@ -20462,7 +20463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="388" spans="1:16">
+    <row r="388" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A388" s="6">
         <v>1</v>
       </c>
@@ -20512,7 +20513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="389" spans="1:16">
+    <row r="389" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A389" s="6">
         <v>1</v>
       </c>
@@ -20562,7 +20563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="390" spans="1:16">
+    <row r="390" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A390" s="6">
         <v>1</v>
       </c>
@@ -20612,7 +20613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="391" spans="1:16">
+    <row r="391" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A391" s="6">
         <v>1</v>
       </c>
@@ -20662,7 +20663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="392" spans="1:16">
+    <row r="392" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A392" s="6">
         <v>1</v>
       </c>
@@ -20712,7 +20713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="393" spans="1:16">
+    <row r="393" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A393" s="6">
         <v>1</v>
       </c>
@@ -20762,7 +20763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="394" spans="1:16">
+    <row r="394" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A394" s="6">
         <v>1</v>
       </c>
@@ -20812,7 +20813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="395" spans="1:16">
+    <row r="395" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A395" s="6">
         <v>1</v>
       </c>
@@ -20862,7 +20863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="396" spans="1:16">
+    <row r="396" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A396" s="6">
         <v>1</v>
       </c>
@@ -20912,7 +20913,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="397" spans="1:16">
+    <row r="397" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A397" s="6">
         <v>1</v>
       </c>
@@ -20962,7 +20963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="398" spans="1:16">
+    <row r="398" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A398" s="6">
         <v>1</v>
       </c>
@@ -21012,7 +21013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="399" spans="1:16">
+    <row r="399" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A399" s="6">
         <v>1</v>
       </c>
@@ -21062,7 +21063,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="400" spans="1:16">
+    <row r="400" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A400" s="6">
         <v>1</v>
       </c>
@@ -21112,7 +21113,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="401" spans="1:16">
+    <row r="401" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A401" s="6">
         <v>1</v>
       </c>
@@ -21162,7 +21163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="402" spans="1:16">
+    <row r="402" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A402" s="7">
         <v>1</v>
       </c>
@@ -21222,34 +21223,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -21299,7 +21300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -21349,7 +21350,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -21399,7 +21400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -21449,7 +21450,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -21499,7 +21500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -21549,7 +21550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -21599,7 +21600,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -21649,7 +21650,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -21699,7 +21700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -21749,7 +21750,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -21799,7 +21800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -21849,7 +21850,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -21899,7 +21900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -21949,7 +21950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -21999,7 +22000,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -22049,7 +22050,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -22099,7 +22100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -22149,7 +22150,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -22199,7 +22200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -22249,7 +22250,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -22299,7 +22300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -22349,7 +22350,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -22399,7 +22400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -22449,7 +22450,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -22499,7 +22500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -22549,7 +22550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
ModelCoverage turned to a parameter table but only indexing regions. This revision is made for the scaling up/down in new construction logic.
</commit_message>
<xml_diff>
--- a/projects/test_building/input/SimulatorScenarios.xlsx
+++ b/projects/test_building/input/SimulatorScenarios.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2F7CA1-2628-144C-A155-780BA156BDEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139DFD7A-2C3B-154D-870B-D5BE4480EB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="-19020" windowWidth="26240" windowHeight="17700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="nuts3" sheetId="1" r:id="rId1"/>
-    <sheet name="test" sheetId="2" r:id="rId2"/>
+    <sheet name="test" sheetId="2" r:id="rId1"/>
+    <sheet name="nuts3" sheetId="1" r:id="rId2"/>
     <sheet name="test-Hessen" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -186,160 +186,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="34">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color rgb="FF8FAADC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF8FAADC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color rgb="FF8FAADC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF8FAADC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color rgb="FF8FAADC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF8FAADC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -541,6 +387,160 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color rgb="FF8FAADC"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF8FAADC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color rgb="FF8FAADC"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF8FAADC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color rgb="FF8FAADC"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF8FAADC"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -623,48 +623,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:O402" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:O402" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:O2" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:O2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="start_year" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="end_year" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="id_region" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{A61F4543-44BF-804C-9854-1F36358A5A9C}" name="id_scenario_teleworking" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="renovation_mandatory" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="heating_technology_mandatory" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="name" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="comment" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="start_year" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="end_year" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_region" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{39CEAB76-A582-8943-9B28-1245EAD02E50}" name="id_scenario_teleworking" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="renovation_mandatory" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="heating_technology_mandatory" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="name" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:O2" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
-  <autoFilter ref="A1:O2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:O402" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A1:O402" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="start_year" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="end_year" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_region" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{39CEAB76-A582-8943-9B28-1245EAD02E50}" name="id_scenario_teleworking" dataDxfId="21"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="renovation_mandatory" dataDxfId="20"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="heating_technology_mandatory" dataDxfId="19"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="name" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="comment" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="start_year" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="end_year" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="id_region" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="optimal_heating_behavior_prob" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="id_scenario_energy_price_wholesale" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="id_scenario_energy_price_tax_rate" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="id_scenario_energy_price_mark_up" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="id_scenario_energy_price_co2_emission" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="id_scenario_energy_emission_factor" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{A61F4543-44BF-804C-9854-1F36358A5A9C}" name="id_scenario_teleworking" dataDxfId="21"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="renovation_mandatory" dataDxfId="20"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="heating_technology_mandatory" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="name" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="comment" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -956,11 +956,141 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.5" customWidth="1"/>
+    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>2019</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2019</v>
+      </c>
+      <c r="D2" s="6">
+        <v>9010101</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O402"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19878,136 +20008,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.5" customWidth="1"/>
-    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6">
-        <v>2019</v>
-      </c>
-      <c r="C2" s="6">
-        <v>2019</v>
-      </c>
-      <c r="D2" s="6">
-        <v>9010101</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="F2" s="6">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6">
-        <v>1</v>
-      </c>
-      <c r="H2" s="6">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6">
-        <v>1</v>
-      </c>
-      <c r="J2" s="6">
-        <v>1</v>
-      </c>
-      <c r="K2" s="6">
-        <v>1</v>
-      </c>
-      <c r="L2" s="4">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
2009 values are added to the two infrastructure available tables
</commit_message>
<xml_diff>
--- a/projects/test_building/input/SimulatorScenarios.xlsx
+++ b/projects/test_building/input/SimulatorScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500BE29B-E027-3D43-ACE4-A4E9592F8149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71B7E45-3024-5945-8CDE-8D5C0E325ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37860" yWindow="-18960" windowWidth="26240" windowHeight="17700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -960,7 +960,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1037,7 +1037,7 @@
         <v>2010</v>
       </c>
       <c r="C2" s="6">
-        <v>2010</v>
+        <v>2050</v>
       </c>
       <c r="D2" s="6">
         <v>9010101</v>

</xml_diff>

<commit_message>
building ownership extended to 2050
</commit_message>
<xml_diff>
--- a/projects/test_building/input/SimulatorScenarios.xlsx
+++ b/projects/test_building/input/SimulatorScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82F4176-96BE-5D41-8A7D-0C55812975FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AFAF4C-5B66-8544-BD59-8B6A3806D809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-40720" yWindow="-19040" windowWidth="26240" windowHeight="17700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -219,6 +219,22 @@
   </cellStyles>
   <dxfs count="26">
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -245,22 +261,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -632,14 +632,14 @@
     <tableColumn id="6" xr3:uid="{6E085763-6428-8849-926E-58D399BA3E52}" name="id_scenario_dh_availability" dataDxfId="10"/>
     <tableColumn id="17" xr3:uid="{F607CC92-C860-4342-92C5-3654F72FFC55}" name="id_scenario_gas_availability" dataDxfId="9"/>
     <tableColumn id="20" xr3:uid="{A0210A8C-0F42-2542-A661-790D5687D85B}" name="id_scenario_hydrogen_availability" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{3018A588-A851-E442-BC12-487FD51F83A5}" name="id_scenario_subsidy_building_renovation" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{9FAD53A0-957A-DE4E-882D-7BCFD06970FE}" name="id_scenario_subsidy_heating_modernization" dataDxfId="0"/>
-    <tableColumn id="18" xr3:uid="{E3BC392B-08E5-6342-825C-FA6099E74527}" name="id_scenario_renovation_mandatory" dataDxfId="7"/>
-    <tableColumn id="19" xr3:uid="{7C3F4DB9-647C-4A42-B5AA-DD0A60CE71A6}" name="id_scenario_heating_technology_mandatory" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="renovation_mandatory" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="heating_technology_mandatory" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="name" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="comment" dataDxfId="2"/>
+    <tableColumn id="23" xr3:uid="{3018A588-A851-E442-BC12-487FD51F83A5}" name="id_scenario_subsidy_building_renovation" dataDxfId="7"/>
+    <tableColumn id="24" xr3:uid="{9FAD53A0-957A-DE4E-882D-7BCFD06970FE}" name="id_scenario_subsidy_heating_modernization" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{E3BC392B-08E5-6342-825C-FA6099E74527}" name="id_scenario_renovation_mandatory" dataDxfId="5"/>
+    <tableColumn id="19" xr3:uid="{7C3F4DB9-647C-4A42-B5AA-DD0A60CE71A6}" name="id_scenario_heating_technology_mandatory" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="renovation_mandatory" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="heating_technology_mandatory" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="name" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -944,7 +944,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1045,7 +1045,7 @@
         <v>2010</v>
       </c>
       <c r="C2">
-        <v>2020</v>
+        <v>2050</v>
       </c>
       <c r="D2">
         <v>9010101</v>

</xml_diff>